<commit_message>
Pielabots par FlagText/FreeText MLVV/LLVV.
</commit_message>
<xml_diff>
--- a/docs/struktuura.xlsx
+++ b/docs/struktuura.xlsx
@@ -3775,7 +3775,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6426,8 +6426,8 @@
       <c r="R54" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="S54" s="4" t="s">
-        <v>132</v>
+      <c r="S54" s="3" t="s">
+        <v>342</v>
       </c>
       <c r="T54" s="9" t="s">
         <v>144</v>
@@ -7364,11 +7364,11 @@
       <c r="Q73" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="R73" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="S73" s="3" t="s">
+      <c r="R73" s="3" t="s">
         <v>359</v>
+      </c>
+      <c r="S73" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="T73" s="9" t="s">
         <v>332</v>
@@ -7408,11 +7408,11 @@
       <c r="Q74" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="R74" s="3" t="s">
+      <c r="R74" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="S74" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="S74" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="T74" s="9" t="s">
         <v>333</v>

</xml_diff>

<commit_message>
Izlabots, ka MLVV vairs nav nozīmes nianses frāžu nozīmēs iekšā.
</commit_message>
<xml_diff>
--- a/docs/struktuura.xlsx
+++ b/docs/struktuura.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4688" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4658" uniqueCount="520">
   <si>
     <t>&gt; python scripts/struktuura.py dati/analyzed_tezaurs.json</t>
   </si>
@@ -2660,12 +2660,6 @@
     <t>Nav, bet visticamāk drīkstētu: ∀ Sample: ≤ 1</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Strukturāla kļūda vārdnīcā vai datu izgūšanā, manuāli jāpārskata un jāsalabo.</t>
-  </si>
-  <si>
     <t>Šķirkļa nozīmes nianšu bloks.</t>
   </si>
   <si>
@@ -2877,9 +2871,6 @@
   </si>
   <si>
     <t>Savienojumi ir divu tipu: "Stabils savienojums", "Frazeoloģisms".</t>
-  </si>
-  <si>
-    <t>Skaidrota nozīmes nianse? Teorētiski skatā pret nākotni, kur frāzes ir šķirkļi, tas būtu pieļaujams… Bet šī ir viena vienīga vieta. Jāpārskata, kas tur ir noticis, un pagaidām jāatrunā MLVV cilvēki no šāda viena izņēmuma.</t>
   </si>
   <si>
     <t>Derivatives</t>
@@ -3619,11 +3610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y267"/>
+  <dimension ref="A1:Y265"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A229" sqref="A229:XFD230"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R142" sqref="R142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3674,10 +3665,10 @@
         <v>107</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>346</v>
@@ -3759,7 +3750,7 @@
         <v>108</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>385</v>
@@ -3791,7 +3782,7 @@
         <v>306</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>385</v>
@@ -3876,7 +3867,7 @@
         <v>145</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>332</v>
@@ -3911,7 +3902,7 @@
         <v>110</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>334</v>
@@ -3961,7 +3952,7 @@
         <v>147</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>333</v>
@@ -4211,7 +4202,7 @@
         <v>383</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>132</v>
@@ -4261,10 +4252,10 @@
         <v>92</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>132</v>
@@ -4308,7 +4299,7 @@
         <v>110</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>335</v>
@@ -4358,7 +4349,7 @@
         <v>175</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>337</v>
@@ -4405,7 +4396,7 @@
         <v>145</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q17" s="4" t="s">
         <v>132</v>
@@ -4452,7 +4443,7 @@
         <v>145</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>338</v>
@@ -4502,7 +4493,7 @@
         <v>110</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q19" s="8" t="s">
         <v>335</v>
@@ -4555,7 +4546,7 @@
         <v>145</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>339</v>
@@ -4697,7 +4688,7 @@
         <v>145</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>341</v>
@@ -4741,7 +4732,7 @@
         <v>110</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>196</v>
@@ -4788,7 +4779,7 @@
         <v>147</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>196</v>
@@ -4879,7 +4870,7 @@
         <v>145</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q27" s="4" t="s">
         <v>132</v>
@@ -4935,7 +4926,7 @@
         <v>145</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q28" s="4" t="s">
         <v>132</v>
@@ -4991,7 +4982,7 @@
         <v>145</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q29" s="4" t="s">
         <v>132</v>
@@ -5047,7 +5038,7 @@
         <v>110</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>335</v>
@@ -5106,7 +5097,7 @@
         <v>175</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>337</v>
@@ -5348,7 +5339,7 @@
         <v>383</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>132</v>
@@ -5407,10 +5398,10 @@
         <v>92</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>132</v>
@@ -5557,7 +5548,7 @@
         <v>145</v>
       </c>
       <c r="P39" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Q39" s="4" t="s">
         <v>132</v>
@@ -5616,7 +5607,7 @@
         <v>145</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q40" s="4" t="s">
         <v>132</v>
@@ -5733,7 +5724,7 @@
         <v>306</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>410</v>
@@ -5976,7 +5967,7 @@
         <v>383</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R48" s="4" t="s">
         <v>132</v>
@@ -6029,10 +6020,10 @@
         <v>92</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R49" s="4" t="s">
         <v>132</v>
@@ -6079,7 +6070,7 @@
         <v>110</v>
       </c>
       <c r="P50" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q50" s="8" t="s">
         <v>297</v>
@@ -6126,7 +6117,7 @@
         <v>175</v>
       </c>
       <c r="P51" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>337</v>
@@ -6172,7 +6163,7 @@
         <v>145</v>
       </c>
       <c r="P52" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q52" s="4" t="s">
         <v>132</v>
@@ -6222,7 +6213,7 @@
         <v>145</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q53" s="3" t="s">
         <v>338</v>
@@ -6275,7 +6266,7 @@
         <v>110</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q54" s="3" t="s">
         <v>335</v>
@@ -6331,7 +6322,7 @@
         <v>145</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>339</v>
@@ -6434,7 +6425,7 @@
         <v>145</v>
       </c>
       <c r="P57" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Q57" s="4" t="s">
         <v>132</v>
@@ -6487,7 +6478,7 @@
         <v>145</v>
       </c>
       <c r="P58" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q58" s="4" t="s">
         <v>132</v>
@@ -6640,7 +6631,7 @@
         <v>145</v>
       </c>
       <c r="P61" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Q61" s="4" t="s">
         <v>132</v>
@@ -6696,7 +6687,7 @@
         <v>110</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Q62" s="4" t="s">
         <v>301</v>
@@ -6749,7 +6740,7 @@
         <v>147</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Q63" s="4" t="s">
         <v>301</v>
@@ -6799,7 +6790,7 @@
         <v>145</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q64" s="4" t="s">
         <v>132</v>
@@ -6931,7 +6922,7 @@
         <v>145</v>
       </c>
       <c r="P67" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q67" s="4" t="s">
         <v>132</v>
@@ -6981,7 +6972,7 @@
         <v>145</v>
       </c>
       <c r="P68" s="6" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="Q68" s="3" t="s">
         <v>353</v>
@@ -7040,7 +7031,7 @@
         <v>354</v>
       </c>
       <c r="T69" s="9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="W69" s="3" t="s">
         <v>377</v>
@@ -7163,7 +7154,7 @@
         <v>145</v>
       </c>
       <c r="P72" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q72" s="4" t="s">
         <v>132</v>
@@ -7207,7 +7198,7 @@
         <v>145</v>
       </c>
       <c r="P73" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q73" s="4" t="s">
         <v>132</v>
@@ -7254,7 +7245,7 @@
         <v>145</v>
       </c>
       <c r="P74" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q74" s="4" t="s">
         <v>132</v>
@@ -7304,7 +7295,7 @@
         <v>145</v>
       </c>
       <c r="P75" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="Q75" s="4" t="s">
         <v>132</v>
@@ -7539,7 +7530,7 @@
         <v>145</v>
       </c>
       <c r="P80" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q80" s="4" t="s">
         <v>132</v>
@@ -7595,7 +7586,7 @@
         <v>145</v>
       </c>
       <c r="P81" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q81" s="4" t="s">
         <v>132</v>
@@ -7648,7 +7639,7 @@
         <v>110</v>
       </c>
       <c r="P82" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q82" s="3" t="s">
         <v>297</v>
@@ -7698,7 +7689,7 @@
         <v>175</v>
       </c>
       <c r="P83" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q83" s="3" t="s">
         <v>297</v>
@@ -7934,7 +7925,7 @@
         <v>383</v>
       </c>
       <c r="Q87" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R87" s="4" t="s">
         <v>132</v>
@@ -7993,10 +7984,10 @@
         <v>92</v>
       </c>
       <c r="P88" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q88" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R88" s="4" t="s">
         <v>132</v>
@@ -8046,7 +8037,7 @@
         <v>230</v>
       </c>
       <c r="P89" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q89" s="3" t="s">
         <v>384</v>
@@ -8061,7 +8052,7 @@
         <v>419</v>
       </c>
       <c r="U89" s="8" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="X89" s="6" t="s">
         <v>402</v>
@@ -8096,7 +8087,7 @@
         <v>145</v>
       </c>
       <c r="P90" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q90" s="3" t="s">
         <v>404</v>
@@ -8123,7 +8114,7 @@
         <v>106</v>
       </c>
       <c r="Y90" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="91" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -8152,7 +8143,7 @@
         <v>145</v>
       </c>
       <c r="P91" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q91" s="4" t="s">
         <v>132</v>
@@ -8202,13 +8193,13 @@
         <v>132</v>
       </c>
       <c r="R92" s="3" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="S92" s="4" t="s">
         <v>132</v>
       </c>
       <c r="T92" s="9" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="X92" s="6" t="s">
         <v>120</v>
@@ -8337,7 +8328,7 @@
         <v>306</v>
       </c>
       <c r="P95" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q95" s="3" t="s">
         <v>412</v>
@@ -8443,7 +8434,7 @@
         <v>145</v>
       </c>
       <c r="P97" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q97" s="4" t="s">
         <v>132</v>
@@ -8502,7 +8493,7 @@
         <v>145</v>
       </c>
       <c r="P98" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q98" s="3" t="s">
         <v>416</v>
@@ -8766,7 +8757,7 @@
         <v>383</v>
       </c>
       <c r="Q102" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R102" s="4" t="s">
         <v>132</v>
@@ -8831,10 +8822,10 @@
         <v>92</v>
       </c>
       <c r="P103" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q103" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R103" s="4" t="s">
         <v>132</v>
@@ -9002,7 +8993,7 @@
         <v>145</v>
       </c>
       <c r="P106" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q106" s="4" t="s">
         <v>132</v>
@@ -9064,7 +9055,7 @@
         <v>145</v>
       </c>
       <c r="P107" s="6" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="Q107" s="3" t="s">
         <v>353</v>
@@ -9135,7 +9126,7 @@
         <v>354</v>
       </c>
       <c r="T108" s="9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="W108" s="3" t="s">
         <v>377</v>
@@ -9294,7 +9285,7 @@
         <v>145</v>
       </c>
       <c r="P111" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q111" s="4" t="s">
         <v>132</v>
@@ -9350,7 +9341,7 @@
         <v>145</v>
       </c>
       <c r="P112" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q112" s="4" t="s">
         <v>132</v>
@@ -9409,7 +9400,7 @@
         <v>145</v>
       </c>
       <c r="P113" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q113" s="4" t="s">
         <v>132</v>
@@ -9471,7 +9462,7 @@
         <v>145</v>
       </c>
       <c r="P114" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="Q114" s="4" t="s">
         <v>132</v>
@@ -9524,7 +9515,7 @@
         <v>354</v>
       </c>
       <c r="T115" s="9" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="X115" s="6" t="s">
         <v>120</v>
@@ -9565,7 +9556,7 @@
         <v>345</v>
       </c>
       <c r="T116" s="9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="X116" s="6" t="s">
         <v>120</v>
@@ -9600,7 +9591,7 @@
         <v>266</v>
       </c>
       <c r="T117" s="9" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="X117" s="6" t="s">
         <v>120</v>
@@ -9647,7 +9638,7 @@
         <v>132</v>
       </c>
       <c r="T118" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="U118" s="11" t="s">
         <v>287</v>
@@ -9821,7 +9812,7 @@
         <v>383</v>
       </c>
       <c r="Q121" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R121" s="4" t="s">
         <v>132</v>
@@ -9880,10 +9871,10 @@
         <v>92</v>
       </c>
       <c r="P122" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q122" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R122" s="4" t="s">
         <v>132</v>
@@ -9936,7 +9927,7 @@
         <v>110</v>
       </c>
       <c r="P123" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q123" s="8" t="s">
         <v>297</v>
@@ -9951,7 +9942,7 @@
         <v>288</v>
       </c>
       <c r="U123" s="8" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="X123" s="6" t="s">
         <v>290</v>
@@ -9989,7 +9980,7 @@
         <v>175</v>
       </c>
       <c r="P124" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q124" s="3" t="s">
         <v>337</v>
@@ -10041,7 +10032,7 @@
         <v>145</v>
       </c>
       <c r="P125" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q125" s="4" t="s">
         <v>132</v>
@@ -10097,7 +10088,7 @@
         <v>145</v>
       </c>
       <c r="P126" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q126" s="3" t="s">
         <v>338</v>
@@ -10112,7 +10103,7 @@
         <v>144</v>
       </c>
       <c r="U126" s="8" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="V126" s="8" t="s">
         <v>293</v>
@@ -10156,7 +10147,7 @@
         <v>110</v>
       </c>
       <c r="P127" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q127" s="3" t="s">
         <v>335</v>
@@ -10218,7 +10209,7 @@
         <v>145</v>
       </c>
       <c r="P128" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q128" s="3" t="s">
         <v>339</v>
@@ -10284,13 +10275,13 @@
         <v>132</v>
       </c>
       <c r="T129" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="V129" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="X129" s="13" t="s">
         <v>445</v>
-      </c>
-      <c r="V129" s="8" t="s">
-        <v>446</v>
-      </c>
-      <c r="X129" s="13" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="130" spans="1:25" x14ac:dyDescent="0.25">
@@ -10337,7 +10328,7 @@
         <v>132</v>
       </c>
       <c r="T130" s="9" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="U130" s="10"/>
       <c r="V130" s="10" t="s">
@@ -10395,7 +10386,7 @@
         <v>132</v>
       </c>
       <c r="T131" s="9" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="V131" s="10"/>
       <c r="X131" s="12" t="s">
@@ -10437,7 +10428,7 @@
         <v>110</v>
       </c>
       <c r="P132" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q132" s="4" t="s">
         <v>132</v>
@@ -10493,7 +10484,7 @@
         <v>147</v>
       </c>
       <c r="P133" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q133" s="4" t="s">
         <v>132</v>
@@ -10602,7 +10593,7 @@
         <v>145</v>
       </c>
       <c r="P135" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q135" s="4" t="s">
         <v>132</v>
@@ -10661,7 +10652,7 @@
         <v>145</v>
       </c>
       <c r="P136" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q136" s="4" t="s">
         <v>132</v>
@@ -10723,7 +10714,7 @@
         <v>132</v>
       </c>
       <c r="T137" s="9" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="U137" s="11" t="s">
         <v>217</v>
@@ -10832,7 +10823,7 @@
         <v>145</v>
       </c>
       <c r="P139" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Q139" s="4" t="s">
         <v>132</v>
@@ -10894,7 +10885,7 @@
         <v>110</v>
       </c>
       <c r="P140" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q140" s="4" t="s">
         <v>301</v>
@@ -10953,7 +10944,7 @@
         <v>147</v>
       </c>
       <c r="P141" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q141" s="4" t="s">
         <v>301</v>
@@ -10965,7 +10956,7 @@
         <v>333</v>
       </c>
       <c r="T141" s="9" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="X141" s="12" t="s">
         <v>106</v>
@@ -11009,7 +11000,7 @@
         <v>145</v>
       </c>
       <c r="P142" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q142" s="4" t="s">
         <v>132</v>
@@ -11021,10 +11012,10 @@
         <v>132</v>
       </c>
       <c r="T142" s="9" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="X142" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="Y142" s="3" t="s">
         <v>201</v>
@@ -11068,7 +11059,7 @@
         <v>145</v>
       </c>
       <c r="P143" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q143" s="4" t="s">
         <v>132</v>
@@ -11130,7 +11121,7 @@
         <v>349</v>
       </c>
       <c r="T144" s="9" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="X144" s="6" t="s">
         <v>120</v>
@@ -11218,7 +11209,7 @@
         <v>145</v>
       </c>
       <c r="P146" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q146" s="4" t="s">
         <v>132</v>
@@ -11274,7 +11265,7 @@
         <v>145</v>
       </c>
       <c r="P147" s="6" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="Q147" s="3" t="s">
         <v>353</v>
@@ -11286,7 +11277,7 @@
         <v>353</v>
       </c>
       <c r="T147" s="9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="U147" s="8" t="s">
         <v>312</v>
@@ -11339,7 +11330,7 @@
         <v>354</v>
       </c>
       <c r="T148" s="9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="W148" s="3" t="s">
         <v>377</v>
@@ -11480,7 +11471,7 @@
         <v>145</v>
       </c>
       <c r="P151" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q151" s="4" t="s">
         <v>132</v>
@@ -11530,7 +11521,7 @@
         <v>145</v>
       </c>
       <c r="P152" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q152" s="4" t="s">
         <v>132</v>
@@ -11639,7 +11630,7 @@
         <v>145</v>
       </c>
       <c r="P154" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="Q154" s="4" t="s">
         <v>132</v>
@@ -11698,7 +11689,7 @@
         <v>354</v>
       </c>
       <c r="T155" s="9" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="U155" s="8" t="s">
         <v>374</v>
@@ -11904,7 +11895,7 @@
         <v>145</v>
       </c>
       <c r="P159" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q159" s="4" t="s">
         <v>132</v>
@@ -11966,7 +11957,7 @@
         <v>145</v>
       </c>
       <c r="P160" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q160" s="4" t="s">
         <v>132</v>
@@ -12227,7 +12218,7 @@
         <v>383</v>
       </c>
       <c r="Q164" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R164" s="4" t="s">
         <v>132</v>
@@ -12292,10 +12283,10 @@
         <v>92</v>
       </c>
       <c r="P165" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q165" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R165" s="4" t="s">
         <v>132</v>
@@ -12351,7 +12342,7 @@
         <v>230</v>
       </c>
       <c r="P166" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q166" s="3" t="s">
         <v>384</v>
@@ -12366,7 +12357,7 @@
         <v>419</v>
       </c>
       <c r="U166" s="8" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="X166" s="6" t="s">
         <v>402</v>
@@ -12407,7 +12398,7 @@
         <v>145</v>
       </c>
       <c r="P167" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q167" s="3" t="s">
         <v>404</v>
@@ -12434,7 +12425,7 @@
         <v>106</v>
       </c>
       <c r="Y167" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="168" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -12469,7 +12460,7 @@
         <v>145</v>
       </c>
       <c r="P168" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q168" s="4" t="s">
         <v>132</v>
@@ -12525,13 +12516,13 @@
         <v>132</v>
       </c>
       <c r="R169" s="3" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="S169" s="4" t="s">
         <v>132</v>
       </c>
       <c r="T169" s="9" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="X169" s="6" t="s">
         <v>120</v>
@@ -12678,7 +12669,7 @@
         <v>306</v>
       </c>
       <c r="P172" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q172" s="3" t="s">
         <v>412</v>
@@ -12796,7 +12787,7 @@
         <v>145</v>
       </c>
       <c r="P174" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q174" s="4" t="s">
         <v>132</v>
@@ -12861,7 +12852,7 @@
         <v>145</v>
       </c>
       <c r="P175" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q175" s="3" t="s">
         <v>335</v>
@@ -13144,7 +13135,7 @@
         <v>383</v>
       </c>
       <c r="Q179" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R179" s="4" t="s">
         <v>132</v>
@@ -13215,10 +13206,10 @@
         <v>92</v>
       </c>
       <c r="P180" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q180" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R180" s="4" t="s">
         <v>132</v>
@@ -13404,7 +13395,7 @@
         <v>145</v>
       </c>
       <c r="P183" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q183" s="4" t="s">
         <v>132</v>
@@ -13413,13 +13404,13 @@
         <v>132</v>
       </c>
       <c r="S183" s="8" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="T183" s="9" t="s">
         <v>315</v>
       </c>
       <c r="W183" s="8" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="X183" s="6" t="s">
         <v>120</v>
@@ -13543,13 +13534,13 @@
         <v>132</v>
       </c>
       <c r="R185" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="S185" s="3" t="s">
         <v>354</v>
       </c>
       <c r="T185" s="9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="W185" s="3"/>
       <c r="X185" s="6" t="s">
@@ -13665,19 +13656,19 @@
         <v>132</v>
       </c>
       <c r="R187" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="S187" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="T187" s="9" t="s">
         <v>425</v>
       </c>
       <c r="V187" s="8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="W187" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="X187" s="13" t="s">
         <v>120</v>
@@ -13730,7 +13721,7 @@
         <v>145</v>
       </c>
       <c r="P188" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q188" s="4" t="s">
         <v>132</v>
@@ -13798,7 +13789,7 @@
         <v>145</v>
       </c>
       <c r="P189" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q189" s="4" t="s">
         <v>132</v>
@@ -13863,7 +13854,7 @@
         <v>145</v>
       </c>
       <c r="P190" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q190" s="4" t="s">
         <v>132</v>
@@ -13931,7 +13922,7 @@
         <v>145</v>
       </c>
       <c r="P191" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="Q191" s="4" t="s">
         <v>132</v>
@@ -13981,16 +13972,16 @@
         <v>344</v>
       </c>
       <c r="T192" s="9" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="U192" s="8" t="s">
         <v>374</v>
       </c>
       <c r="V192" s="8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="W192" s="8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="X192" s="6" t="s">
         <v>120</v>
@@ -14025,7 +14016,7 @@
         <v>380</v>
       </c>
       <c r="T193" s="9" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="X193" s="6" t="s">
         <v>120</v>
@@ -14063,16 +14054,16 @@
         <v>384</v>
       </c>
       <c r="T194" s="9" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="U194" s="8" t="s">
         <v>388</v>
       </c>
       <c r="V194" s="8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="W194" s="8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="X194" s="6" t="s">
         <v>120</v>
@@ -14139,7 +14130,7 @@
         <v>145</v>
       </c>
       <c r="P196" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q196" s="4" t="s">
         <v>132</v>
@@ -14189,7 +14180,7 @@
         <v>145</v>
       </c>
       <c r="P197" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q197" s="4" t="s">
         <v>132</v>
@@ -14236,7 +14227,7 @@
         <v>110</v>
       </c>
       <c r="P198" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q198" s="3" t="s">
         <v>297</v>
@@ -14280,7 +14271,7 @@
         <v>175</v>
       </c>
       <c r="P199" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q199" s="3" t="s">
         <v>297</v>
@@ -14492,7 +14483,7 @@
         <v>383</v>
       </c>
       <c r="Q203" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R203" s="4" t="s">
         <v>132</v>
@@ -14545,10 +14536,10 @@
         <v>92</v>
       </c>
       <c r="P204" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q204" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R204" s="4" t="s">
         <v>132</v>
@@ -14592,7 +14583,7 @@
         <v>230</v>
       </c>
       <c r="P205" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q205" s="3" t="s">
         <v>384</v>
@@ -14607,7 +14598,7 @@
         <v>419</v>
       </c>
       <c r="U205" s="8" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="X205" s="6" t="s">
         <v>402</v>
@@ -14636,7 +14627,7 @@
         <v>145</v>
       </c>
       <c r="P206" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q206" s="3" t="s">
         <v>404</v>
@@ -14663,7 +14654,7 @@
         <v>106</v>
       </c>
       <c r="Y206" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="207" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -14771,7 +14762,7 @@
         <v>306</v>
       </c>
       <c r="P209" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Q209" s="3" t="s">
         <v>412</v>
@@ -14865,7 +14856,7 @@
         <v>145</v>
       </c>
       <c r="P211" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q211" s="4" t="s">
         <v>132</v>
@@ -14918,7 +14909,7 @@
         <v>145</v>
       </c>
       <c r="P212" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q212" s="3" t="s">
         <v>335</v>
@@ -15158,7 +15149,7 @@
         <v>383</v>
       </c>
       <c r="Q216" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R216" s="4" t="s">
         <v>132</v>
@@ -15217,10 +15208,10 @@
         <v>92</v>
       </c>
       <c r="P217" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q217" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R217" s="4" t="s">
         <v>132</v>
@@ -15370,7 +15361,7 @@
         <v>145</v>
       </c>
       <c r="P220" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q220" s="4" t="s">
         <v>132</v>
@@ -15426,7 +15417,7 @@
         <v>145</v>
       </c>
       <c r="P221" s="6" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="Q221" s="3" t="s">
         <v>353</v>
@@ -15491,7 +15482,7 @@
         <v>354</v>
       </c>
       <c r="T222" s="9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="W222" s="3"/>
       <c r="X222" s="6" t="s">
@@ -15583,7 +15574,7 @@
         <v>132</v>
       </c>
       <c r="R224" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="S224" s="3" t="s">
         <v>355</v>
@@ -15592,7 +15583,7 @@
         <v>425</v>
       </c>
       <c r="V224" s="8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="X224" s="13" t="s">
         <v>120</v>
@@ -15633,7 +15624,7 @@
         <v>145</v>
       </c>
       <c r="P225" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q225" s="4" t="s">
         <v>132</v>
@@ -15689,7 +15680,7 @@
         <v>145</v>
       </c>
       <c r="P226" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q226" s="4" t="s">
         <v>132</v>
@@ -15742,7 +15733,7 @@
         <v>145</v>
       </c>
       <c r="P227" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q227" s="4" t="s">
         <v>132</v>
@@ -15798,7 +15789,7 @@
         <v>145</v>
       </c>
       <c r="P228" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="Q228" s="4" t="s">
         <v>132</v>
@@ -15827,72 +15818,51 @@
         <v>180</v>
       </c>
       <c r="B229" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="C229" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="D229" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="E229" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="F229" s="15" t="s">
-        <v>224</v>
+        <v>468</v>
       </c>
       <c r="N229" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O229" s="6" t="s">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="P229" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="Q229" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="R229" s="3" t="s">
-        <v>297</v>
+      <c r="Q229" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="R229" s="8" t="s">
+        <v>344</v>
       </c>
       <c r="S229" s="4" t="s">
         <v>132</v>
       </c>
       <c r="T229" s="9" t="s">
-        <v>429</v>
+        <v>470</v>
+      </c>
+      <c r="U229" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="W229" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="X229" s="6" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="230" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A230" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B230" s="15" t="s">
-        <v>359</v>
+        <v>468</v>
       </c>
       <c r="C230" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="D230" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="E230" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="F230" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="G230" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="H230" s="15" t="s">
-        <v>428</v>
-      </c>
-      <c r="N230" s="7" t="s">
-        <v>132</v>
+        <v>104</v>
+      </c>
+      <c r="N230" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="O230" s="6" t="s">
         <v>110</v>
@@ -15900,20 +15870,23 @@
       <c r="P230" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="Q230" s="4" t="s">
-        <v>132</v>
+      <c r="Q230" s="3" t="s">
+        <v>469</v>
       </c>
       <c r="R230" s="3" t="s">
-        <v>297</v>
+        <v>469</v>
       </c>
       <c r="S230" s="4" t="s">
         <v>132</v>
       </c>
       <c r="T230" s="9" t="s">
-        <v>470</v>
-      </c>
+        <v>471</v>
+      </c>
+      <c r="U230" s="10"/>
+      <c r="V230" s="10"/>
+      <c r="W230" s="10"/>
       <c r="X230" s="6" t="s">
-        <v>290</v>
+        <v>120</v>
       </c>
     </row>
     <row r="231" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -15921,73 +15894,76 @@
         <v>180</v>
       </c>
       <c r="B231" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="N231" s="7" t="s">
-        <v>225</v>
+        <v>468</v>
+      </c>
+      <c r="C231" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D231" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="N231" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O231" s="6" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="P231" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q231" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="R231" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="S231" s="4" t="s">
-        <v>132</v>
+        <v>502</v>
+      </c>
+      <c r="Q231" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="R231" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="S231" s="3" t="s">
+        <v>341</v>
       </c>
       <c r="T231" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="U231" s="8" t="s">
-        <v>476</v>
-      </c>
-      <c r="W231" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="X231" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B232" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C232" s="15" t="s">
         <v>104</v>
       </c>
+      <c r="D232" s="15" t="s">
+        <v>116</v>
+      </c>
       <c r="N232" s="6" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="O232" s="6" t="s">
         <v>110</v>
       </c>
       <c r="P232" s="6" t="s">
-        <v>266</v>
+        <v>503</v>
       </c>
       <c r="Q232" s="3" t="s">
-        <v>472</v>
+        <v>196</v>
       </c>
       <c r="R232" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="S232" s="4" t="s">
-        <v>132</v>
+        <v>334</v>
+      </c>
+      <c r="S232" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="T232" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="U232" s="10"/>
-      <c r="V232" s="10"/>
-      <c r="W232" s="10"/>
+        <v>475</v>
+      </c>
+      <c r="U232" s="8" t="s">
+        <v>476</v>
+      </c>
       <c r="X232" s="6" t="s">
         <v>120</v>
       </c>
@@ -15997,63 +15973,69 @@
         <v>180</v>
       </c>
       <c r="B233" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C233" s="15" t="s">
         <v>104</v>
       </c>
       <c r="D233" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="N233" s="6" t="s">
-        <v>109</v>
+        <v>116</v>
+      </c>
+      <c r="E233" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="N233" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="O233" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="P233" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="Q233" s="3" t="s">
-        <v>341</v>
+        <v>196</v>
       </c>
       <c r="R233" s="3" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="S233" s="3" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="T233" s="9" t="s">
         <v>477</v>
       </c>
+      <c r="U233" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="X233" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="234" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A234" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B234" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C234" s="15" t="s">
         <v>104</v>
       </c>
       <c r="D234" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N234" s="6" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="O234" s="6" t="s">
         <v>110</v>
       </c>
       <c r="P234" s="6" t="s">
-        <v>506</v>
+        <v>266</v>
       </c>
       <c r="Q234" s="3" t="s">
-        <v>196</v>
+        <v>334</v>
       </c>
       <c r="R234" s="3" t="s">
         <v>334</v>
@@ -16064,10 +16046,7 @@
       <c r="T234" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="U234" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="X234" s="6" t="s">
+      <c r="X234" s="13" t="s">
         <v>120</v>
       </c>
     </row>
@@ -16076,51 +16055,57 @@
         <v>180</v>
       </c>
       <c r="B235" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C235" s="15" t="s">
         <v>104</v>
       </c>
       <c r="D235" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E235" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="N235" s="7" t="s">
-        <v>132</v>
+        <v>202</v>
+      </c>
+      <c r="N235" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O235" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P235" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="Q235" s="3" t="s">
-        <v>196</v>
+        <v>505</v>
+      </c>
+      <c r="Q235" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="R235" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="S235" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
+      </c>
+      <c r="S235" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="T235" s="9" t="s">
-        <v>480</v>
-      </c>
-      <c r="U235" s="10" t="s">
-        <v>106</v>
+        <v>207</v>
+      </c>
+      <c r="U235" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="W235" s="8" t="s">
+        <v>149</v>
       </c>
       <c r="X235" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="236" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y235" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="236" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B236" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C236" s="15" t="s">
         <v>104</v>
@@ -16128,29 +16113,41 @@
       <c r="D236" s="15" t="s">
         <v>114</v>
       </c>
+      <c r="E236" s="15" t="s">
+        <v>148</v>
+      </c>
       <c r="N236" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O236" s="6" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="P236" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q236" s="3" t="s">
-        <v>334</v>
+        <v>505</v>
+      </c>
+      <c r="Q236" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="R236" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="S236" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c r="S236" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="T236" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="X236" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="U236" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="W236" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="X236" s="6" t="s">
         <v>120</v>
+      </c>
+      <c r="Y236" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="237" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -16158,7 +16155,7 @@
         <v>180</v>
       </c>
       <c r="B237" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C237" s="15" t="s">
         <v>104</v>
@@ -16167,7 +16164,7 @@
         <v>114</v>
       </c>
       <c r="E237" s="15" t="s">
-        <v>202</v>
+        <v>142</v>
       </c>
       <c r="N237" s="6" t="s">
         <v>109</v>
@@ -16176,25 +16173,25 @@
         <v>145</v>
       </c>
       <c r="P237" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Q237" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="R237" s="3" t="s">
+      <c r="R237" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="S237" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="S237" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="T237" s="9" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="U237" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="W237" s="8" t="s">
-        <v>149</v>
+        <v>199</v>
+      </c>
+      <c r="V237" s="8" t="s">
+        <v>200</v>
       </c>
       <c r="X237" s="6" t="s">
         <v>120</v>
@@ -16203,12 +16200,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="238" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A238" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B238" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C238" s="15" t="s">
         <v>104</v>
@@ -16217,40 +16214,40 @@
         <v>114</v>
       </c>
       <c r="E238" s="15" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="N238" s="6" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="O238" s="6" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="P238" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="Q238" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="R238" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q238" s="3" t="s">
         <v>335</v>
       </c>
+      <c r="R238" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="S238" s="4" t="s">
         <v>132</v>
       </c>
       <c r="T238" s="9" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="U238" s="8" t="s">
-        <v>205</v>
+        <v>208</v>
+      </c>
+      <c r="V238" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="W238" s="8" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="X238" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y238" s="3" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
     </row>
     <row r="239" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -16258,7 +16255,7 @@
         <v>180</v>
       </c>
       <c r="B239" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C239" s="15" t="s">
         <v>104</v>
@@ -16267,48 +16264,51 @@
         <v>114</v>
       </c>
       <c r="E239" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="N239" s="6" t="s">
-        <v>109</v>
+        <v>163</v>
+      </c>
+      <c r="F239" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="N239" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="O239" s="6" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="P239" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="Q239" s="4" t="s">
-        <v>132</v>
+        <v>501</v>
+      </c>
+      <c r="Q239" s="3" t="s">
+        <v>337</v>
       </c>
       <c r="R239" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="S239" s="3" t="s">
-        <v>335</v>
+      <c r="S239" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="T239" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="U239" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="V239" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="X239" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y239" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="240" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="U239" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="V239" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="W239" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="X239" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="240" spans="1:25" ht="90" x14ac:dyDescent="0.25">
       <c r="A240" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B240" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C240" s="15" t="s">
         <v>104</v>
@@ -16317,16 +16317,16 @@
         <v>114</v>
       </c>
       <c r="E240" s="15" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="N240" s="6" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="O240" s="6" t="s">
         <v>110</v>
       </c>
       <c r="P240" s="6" t="s">
-        <v>504</v>
+        <v>266</v>
       </c>
       <c r="Q240" s="3" t="s">
         <v>335</v>
@@ -16338,10 +16338,10 @@
         <v>132</v>
       </c>
       <c r="T240" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="U240" s="8" t="s">
-        <v>208</v>
+        <v>216</v>
+      </c>
+      <c r="U240" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="V240" s="8" t="s">
         <v>133</v>
@@ -16350,15 +16350,15 @@
         <v>134</v>
       </c>
       <c r="X240" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="241" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="241" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A241" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B241" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C241" s="15" t="s">
         <v>104</v>
@@ -16367,22 +16367,25 @@
         <v>114</v>
       </c>
       <c r="E241" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="F241" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="N241" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="O241" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="P241" s="6" t="s">
-        <v>504</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F241" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G241" s="17"/>
+      <c r="J241" s="17"/>
+      <c r="K241" s="17"/>
+      <c r="L241" s="17"/>
+      <c r="M241" s="17"/>
+      <c r="N241" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="O241" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="P241" s="7"/>
       <c r="Q241" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R241" s="4" t="s">
         <v>132</v>
@@ -16391,7 +16394,7 @@
         <v>132</v>
       </c>
       <c r="T241" s="9" t="s">
-        <v>210</v>
+        <v>135</v>
       </c>
       <c r="U241" s="10" t="s">
         <v>106</v>
@@ -16406,12 +16409,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="242" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A242" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B242" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C242" s="15" t="s">
         <v>104</v>
@@ -16422,8 +16425,11 @@
       <c r="E242" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="N242" s="6" t="s">
-        <v>110</v>
+      <c r="F242" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="N242" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="O242" s="6" t="s">
         <v>110</v>
@@ -16432,7 +16438,7 @@
         <v>266</v>
       </c>
       <c r="Q242" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="R242" s="4" t="s">
         <v>132</v>
@@ -16441,27 +16447,27 @@
         <v>132</v>
       </c>
       <c r="T242" s="9" t="s">
-        <v>216</v>
+        <v>138</v>
       </c>
       <c r="U242" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="V242" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="W242" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="X242" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="243" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+      <c r="V242" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="W242" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="X242" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="243" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A243" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B243" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C243" s="15" t="s">
         <v>104</v>
@@ -16472,23 +16478,23 @@
       <c r="E243" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="F243" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G243" s="17"/>
-      <c r="J243" s="17"/>
-      <c r="K243" s="17"/>
-      <c r="L243" s="17"/>
-      <c r="M243" s="17"/>
-      <c r="N243" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="O243" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="P243" s="7"/>
+      <c r="F243" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G243" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="N243" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O243" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="P243" s="6" t="s">
+        <v>383</v>
+      </c>
       <c r="Q243" s="3" t="s">
-        <v>336</v>
+        <v>456</v>
       </c>
       <c r="R243" s="4" t="s">
         <v>132</v>
@@ -16497,7 +16503,7 @@
         <v>132</v>
       </c>
       <c r="T243" s="9" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="U243" s="10" t="s">
         <v>106</v>
@@ -16512,12 +16518,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A244" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B244" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C244" s="15" t="s">
         <v>104</v>
@@ -16531,17 +16537,20 @@
       <c r="F244" s="15" t="s">
         <v>137</v>
       </c>
+      <c r="G244" s="15" t="s">
+        <v>140</v>
+      </c>
       <c r="N244" s="7" t="s">
         <v>132</v>
       </c>
       <c r="O244" s="6" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="P244" s="6" t="s">
-        <v>266</v>
+        <v>509</v>
       </c>
       <c r="Q244" s="3" t="s">
-        <v>336</v>
+        <v>456</v>
       </c>
       <c r="R244" s="4" t="s">
         <v>132</v>
@@ -16550,7 +16559,7 @@
         <v>132</v>
       </c>
       <c r="T244" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="U244" s="10" t="s">
         <v>106</v>
@@ -16565,12 +16574,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A245" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B245" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C245" s="15" t="s">
         <v>104</v>
@@ -16579,25 +16588,19 @@
         <v>114</v>
       </c>
       <c r="E245" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F245" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G245" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="N245" s="7" t="s">
-        <v>132</v>
+        <v>170</v>
+      </c>
+      <c r="N245" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="O245" s="6" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="P245" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="Q245" s="3" t="s">
-        <v>458</v>
+        <v>504</v>
+      </c>
+      <c r="Q245" s="8" t="s">
+        <v>335</v>
       </c>
       <c r="R245" s="4" t="s">
         <v>132</v>
@@ -16606,10 +16609,10 @@
         <v>132</v>
       </c>
       <c r="T245" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="U245" s="10" t="s">
-        <v>106</v>
+        <v>178</v>
+      </c>
+      <c r="U245" s="11" t="s">
+        <v>177</v>
       </c>
       <c r="V245" s="10" t="s">
         <v>106</v>
@@ -16617,16 +16620,16 @@
       <c r="W245" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="X245" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="246" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="X245" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="246" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B246" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C246" s="15" t="s">
         <v>104</v>
@@ -16635,25 +16638,25 @@
         <v>114</v>
       </c>
       <c r="E246" s="15" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
       <c r="F246" s="15" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="G246" s="15" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="N246" s="7" t="s">
         <v>132</v>
       </c>
       <c r="O246" s="6" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="P246" s="6" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="Q246" s="3" t="s">
-        <v>458</v>
+        <v>339</v>
       </c>
       <c r="R246" s="4" t="s">
         <v>132</v>
@@ -16662,17 +16665,11 @@
         <v>132</v>
       </c>
       <c r="T246" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="U246" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="V246" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="W246" s="10" t="s">
-        <v>106</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="U246" s="10"/>
+      <c r="V246" s="10"/>
+      <c r="W246" s="10"/>
       <c r="X246" s="12" t="s">
         <v>106</v>
       </c>
@@ -16682,7 +16679,7 @@
         <v>180</v>
       </c>
       <c r="B247" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C247" s="15" t="s">
         <v>104</v>
@@ -16691,16 +16688,16 @@
         <v>114</v>
       </c>
       <c r="E247" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="N247" s="6" t="s">
-        <v>171</v>
+        <v>181</v>
+      </c>
+      <c r="N247" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="O247" s="6" t="s">
         <v>110</v>
       </c>
       <c r="P247" s="6" t="s">
-        <v>507</v>
+        <v>266</v>
       </c>
       <c r="Q247" s="8" t="s">
         <v>335</v>
@@ -16712,27 +16709,21 @@
         <v>132</v>
       </c>
       <c r="T247" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="U247" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="V247" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="W247" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="X247" s="13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="248" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+      <c r="U247" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="X247" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A248" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B248" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C248" s="15" t="s">
         <v>104</v>
@@ -16741,25 +16732,22 @@
         <v>114</v>
       </c>
       <c r="E248" s="15" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F248" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="G248" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="N248" s="7" t="s">
-        <v>132</v>
+        <v>104</v>
+      </c>
+      <c r="N248" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="O248" s="6" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="P248" s="6" t="s">
-        <v>507</v>
+        <v>266</v>
       </c>
       <c r="Q248" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="R248" s="4" t="s">
         <v>132</v>
@@ -16768,7 +16756,7 @@
         <v>132</v>
       </c>
       <c r="T248" s="9" t="s">
-        <v>179</v>
+        <v>480</v>
       </c>
       <c r="U248" s="10"/>
       <c r="V248" s="10"/>
@@ -16777,12 +16765,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="249" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B249" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C249" s="15" t="s">
         <v>104</v>
@@ -16793,17 +16781,20 @@
       <c r="E249" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="N249" s="7" t="s">
-        <v>225</v>
+      <c r="F249" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G249" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="N249" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O249" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="P249" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q249" s="8" t="s">
-        <v>335</v>
+        <v>145</v>
+      </c>
+      <c r="Q249" s="3" t="s">
+        <v>341</v>
       </c>
       <c r="R249" s="4" t="s">
         <v>132</v>
@@ -16812,21 +16803,18 @@
         <v>132</v>
       </c>
       <c r="T249" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="U249" s="8" t="s">
-        <v>484</v>
-      </c>
-      <c r="X249" s="6" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="X249" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="250" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A250" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B250" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C250" s="15" t="s">
         <v>104</v>
@@ -16840,17 +16828,20 @@
       <c r="F250" s="15" t="s">
         <v>104</v>
       </c>
+      <c r="G250" s="15" t="s">
+        <v>116</v>
+      </c>
       <c r="N250" s="6" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="O250" s="6" t="s">
         <v>110</v>
       </c>
       <c r="P250" s="6" t="s">
-        <v>266</v>
+        <v>503</v>
       </c>
       <c r="Q250" s="3" t="s">
-        <v>340</v>
+        <v>196</v>
       </c>
       <c r="R250" s="4" t="s">
         <v>132</v>
@@ -16859,13 +16850,13 @@
         <v>132</v>
       </c>
       <c r="T250" s="9" t="s">
-        <v>483</v>
-      </c>
-      <c r="U250" s="10"/>
-      <c r="V250" s="10"/>
-      <c r="W250" s="10"/>
-      <c r="X250" s="12" t="s">
-        <v>106</v>
+        <v>192</v>
+      </c>
+      <c r="U250" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="X250" s="6" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="251" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -16873,7 +16864,7 @@
         <v>180</v>
       </c>
       <c r="B251" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C251" s="15" t="s">
         <v>104</v>
@@ -16888,16 +16879,22 @@
         <v>104</v>
       </c>
       <c r="G251" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="N251" s="6" t="s">
-        <v>109</v>
+        <v>116</v>
+      </c>
+      <c r="H251" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="N251" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="O251" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
+      </c>
+      <c r="P251" s="6" t="s">
+        <v>503</v>
       </c>
       <c r="Q251" s="3" t="s">
-        <v>341</v>
+        <v>196</v>
       </c>
       <c r="R251" s="4" t="s">
         <v>132</v>
@@ -16906,18 +16903,21 @@
         <v>132</v>
       </c>
       <c r="T251" s="9" t="s">
-        <v>191</v>
+        <v>197</v>
+      </c>
+      <c r="U251" s="8" t="s">
+        <v>482</v>
       </c>
       <c r="X251" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="252" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A252" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B252" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C252" s="15" t="s">
         <v>104</v>
@@ -16932,19 +16932,19 @@
         <v>104</v>
       </c>
       <c r="G252" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N252" s="6" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="O252" s="6" t="s">
         <v>110</v>
       </c>
       <c r="P252" s="6" t="s">
-        <v>506</v>
+        <v>266</v>
       </c>
       <c r="Q252" s="3" t="s">
-        <v>196</v>
+        <v>334</v>
       </c>
       <c r="R252" s="4" t="s">
         <v>132</v>
@@ -16953,21 +16953,18 @@
         <v>132</v>
       </c>
       <c r="T252" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="U252" s="8" t="s">
-        <v>485</v>
-      </c>
-      <c r="X252" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="253" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="X252" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="253" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B253" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C253" s="15" t="s">
         <v>104</v>
@@ -16982,22 +16979,22 @@
         <v>104</v>
       </c>
       <c r="G253" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H253" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="N253" s="7" t="s">
-        <v>132</v>
+        <v>163</v>
+      </c>
+      <c r="N253" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="O253" s="6" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="P253" s="6" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="Q253" s="3" t="s">
-        <v>196</v>
+        <v>335</v>
       </c>
       <c r="R253" s="4" t="s">
         <v>132</v>
@@ -17006,21 +17003,21 @@
         <v>132</v>
       </c>
       <c r="T253" s="9" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="U253" s="8" t="s">
-        <v>485</v>
-      </c>
-      <c r="X253" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="X253" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="254" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B254" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C254" s="15" t="s">
         <v>104</v>
@@ -17037,17 +17034,23 @@
       <c r="G254" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="N254" s="6" t="s">
-        <v>110</v>
+      <c r="H254" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I254" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="N254" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="O254" s="6" t="s">
-        <v>110</v>
+        <v>175</v>
       </c>
       <c r="P254" s="6" t="s">
-        <v>266</v>
+        <v>501</v>
       </c>
       <c r="Q254" s="3" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="R254" s="4" t="s">
         <v>132</v>
@@ -17056,18 +17059,23 @@
         <v>132</v>
       </c>
       <c r="T254" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="X254" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="255" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="U254" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="V254" s="10"/>
+      <c r="W254" s="10"/>
+      <c r="X254" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="255" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A255" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B255" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C255" s="15" t="s">
         <v>104</v>
@@ -17085,16 +17093,16 @@
         <v>114</v>
       </c>
       <c r="H255" s="15" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="N255" s="6" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="O255" s="6" t="s">
         <v>110</v>
       </c>
       <c r="P255" s="6" t="s">
-        <v>504</v>
+        <v>266</v>
       </c>
       <c r="Q255" s="3" t="s">
         <v>335</v>
@@ -17106,21 +17114,21 @@
         <v>132</v>
       </c>
       <c r="T255" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="U255" s="8" t="s">
-        <v>208</v>
+        <v>216</v>
+      </c>
+      <c r="U255" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="X255" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="256" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="256" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A256" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B256" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C256" s="15" t="s">
         <v>104</v>
@@ -17138,22 +17146,24 @@
         <v>114</v>
       </c>
       <c r="H256" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="I256" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="N256" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="O256" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="P256" s="6" t="s">
-        <v>504</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="I256" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="J256" s="17"/>
+      <c r="K256" s="17"/>
+      <c r="L256" s="17"/>
+      <c r="M256" s="17"/>
+      <c r="N256" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="O256" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="P256" s="7"/>
       <c r="Q256" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R256" s="4" t="s">
         <v>132</v>
@@ -17162,7 +17172,7 @@
         <v>132</v>
       </c>
       <c r="T256" s="9" t="s">
-        <v>210</v>
+        <v>135</v>
       </c>
       <c r="U256" s="10" t="s">
         <v>106</v>
@@ -17173,12 +17183,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="257" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A257" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B257" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C257" s="15" t="s">
         <v>104</v>
@@ -17198,8 +17208,11 @@
       <c r="H257" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="N257" s="6" t="s">
-        <v>110</v>
+      <c r="I257" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="N257" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="O257" s="6" t="s">
         <v>110</v>
@@ -17208,7 +17221,7 @@
         <v>266</v>
       </c>
       <c r="Q257" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="R257" s="4" t="s">
         <v>132</v>
@@ -17217,21 +17230,23 @@
         <v>132</v>
       </c>
       <c r="T257" s="9" t="s">
-        <v>216</v>
+        <v>138</v>
       </c>
       <c r="U257" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="X257" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="258" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+      <c r="V257" s="10"/>
+      <c r="W257" s="10"/>
+      <c r="X257" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="258" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A258" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B258" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C258" s="15" t="s">
         <v>104</v>
@@ -17251,22 +17266,23 @@
       <c r="H258" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="I258" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="J258" s="17"/>
-      <c r="K258" s="17"/>
-      <c r="L258" s="17"/>
-      <c r="M258" s="17"/>
-      <c r="N258" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="O258" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="P258" s="7"/>
+      <c r="I258" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="J258" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="N258" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O258" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="P258" s="6" t="s">
+        <v>383</v>
+      </c>
       <c r="Q258" s="3" t="s">
-        <v>336</v>
+        <v>456</v>
       </c>
       <c r="R258" s="4" t="s">
         <v>132</v>
@@ -17275,7 +17291,7 @@
         <v>132</v>
       </c>
       <c r="T258" s="9" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="U258" s="10" t="s">
         <v>106</v>
@@ -17286,12 +17302,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A259" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B259" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C259" s="15" t="s">
         <v>104</v>
@@ -17314,17 +17330,20 @@
       <c r="I259" s="15" t="s">
         <v>137</v>
       </c>
+      <c r="J259" s="15" t="s">
+        <v>140</v>
+      </c>
       <c r="N259" s="7" t="s">
         <v>132</v>
       </c>
       <c r="O259" s="6" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="P259" s="6" t="s">
-        <v>266</v>
+        <v>509</v>
       </c>
       <c r="Q259" s="3" t="s">
-        <v>336</v>
+        <v>456</v>
       </c>
       <c r="R259" s="4" t="s">
         <v>132</v>
@@ -17333,7 +17352,7 @@
         <v>132</v>
       </c>
       <c r="T259" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="U259" s="10" t="s">
         <v>106</v>
@@ -17344,143 +17363,91 @@
         <v>106</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B260" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="C260" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D260" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="E260" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="F260" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G260" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="H260" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="I260" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="J260" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="N260" s="7" t="s">
-        <v>132</v>
+        <v>25</v>
+      </c>
+      <c r="N260" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O260" s="6" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="P260" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="Q260" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="R260" s="4" t="s">
-        <v>132</v>
+        <v>513</v>
+      </c>
+      <c r="Q260" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="R260" s="8" t="s">
+        <v>344</v>
       </c>
       <c r="S260" s="4" t="s">
         <v>132</v>
       </c>
       <c r="T260" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="U260" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="V260" s="10"/>
-      <c r="W260" s="10"/>
-      <c r="X260" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="261" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+      <c r="U260" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="V260" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="X260" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="261" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B261" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="C261" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D261" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="E261" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="F261" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G261" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="H261" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="I261" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="J261" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="N261" s="7" t="s">
-        <v>132</v>
+        <v>51</v>
+      </c>
+      <c r="N261" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O261" s="6" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="P261" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="Q261" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="R261" s="4" t="s">
-        <v>132</v>
+        <v>513</v>
+      </c>
+      <c r="Q261" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="R261" s="8" t="s">
+        <v>344</v>
       </c>
       <c r="S261" s="4" t="s">
         <v>132</v>
       </c>
       <c r="T261" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="U261" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="V261" s="10"/>
-      <c r="W261" s="10"/>
-      <c r="X261" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="262" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+      <c r="X261" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="262" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B262" s="15" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="N262" s="6" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="O262" s="6" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="P262" s="6" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="Q262" s="8" t="s">
         <v>344</v>
@@ -17488,60 +17455,60 @@
       <c r="R262" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="S262" s="4" t="s">
-        <v>132</v>
+      <c r="S262" s="8" t="s">
+        <v>344</v>
       </c>
       <c r="T262" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="U262" s="8" t="s">
-        <v>487</v>
-      </c>
-      <c r="V262" s="8" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="X262" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="263" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A263" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B263" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="N263" s="6" t="s">
-        <v>109</v>
+        <v>9</v>
+      </c>
+      <c r="C263" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="N263" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="O263" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="P263" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="Q263" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="R263" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="S263" s="4" t="s">
-        <v>132</v>
+        <v>511</v>
+      </c>
+      <c r="Q263" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="R263" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="S263" s="3" t="s">
+        <v>488</v>
       </c>
       <c r="T263" s="9" t="s">
         <v>489</v>
       </c>
+      <c r="U263" s="8" t="s">
+        <v>491</v>
+      </c>
       <c r="X263" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="264" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B264" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N264" s="6" t="s">
         <v>146</v>
@@ -17550,33 +17517,39 @@
         <v>110</v>
       </c>
       <c r="P264" s="6" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="Q264" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="R264" s="8" t="s">
-        <v>344</v>
+        <v>498</v>
+      </c>
+      <c r="R264" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="S264" s="8" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="T264" s="9" t="s">
-        <v>493</v>
+        <v>496</v>
+      </c>
+      <c r="U264" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="W264" s="8" t="s">
+        <v>499</v>
       </c>
       <c r="X264" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="265" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A265" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B265" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C265" s="15" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="N265" s="7" t="s">
         <v>132</v>
@@ -17585,103 +17558,27 @@
         <v>147</v>
       </c>
       <c r="P265" s="6" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="Q265" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="R265" s="3" t="s">
-        <v>491</v>
+        <v>493</v>
+      </c>
+      <c r="R265" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="S265" s="3" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="T265" s="9" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="U265" s="8" t="s">
-        <v>494</v>
+        <v>512</v>
+      </c>
+      <c r="W265" s="8" t="s">
+        <v>500</v>
       </c>
       <c r="X265" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="266" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A266" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B266" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N266" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="O266" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="P266" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="Q266" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="R266" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="S266" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="T266" s="9" t="s">
-        <v>499</v>
-      </c>
-      <c r="U266" s="8" t="s">
-        <v>497</v>
-      </c>
-      <c r="W266" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="X266" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="267" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A267" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B267" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C267" s="15" t="s">
-        <v>495</v>
-      </c>
-      <c r="N267" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="O267" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="P267" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="Q267" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="R267" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="S267" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="T267" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="U267" s="8" t="s">
-        <v>515</v>
-      </c>
-      <c r="W267" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="X267" s="6" t="s">
         <v>120</v>
       </c>
     </row>
@@ -19427,41 +19324,41 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arī šķirkļa līmeņa frāžu blokā drīkst būt Taksona tipa frāzes (MLVV).
</commit_message>
<xml_diff>
--- a/docs/struktuura.xlsx
+++ b/docs/struktuura.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4591" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4615" uniqueCount="515">
   <si>
     <t>&gt; python scripts/struktuura.py dati/analyzed_tezaurs.json</t>
   </si>
@@ -2798,9 +2798,6 @@
   </si>
   <si>
     <t>Skaidroto vārdus savienojumu bloks,kas nav piesaistīts nevienai nozīmei.</t>
-  </si>
-  <si>
-    <t>Skaidrotā savienojuma tips: "Stabils savienojums", "Frazeoloģisms".</t>
   </si>
   <si>
     <t>Viens skaidrots vārdu savienojums: stabils savienojums ar vai bez nozīmes pārnesuma (Tēzaurā nav dalīts, MLVV un LLVV ir).</t>
@@ -3552,11 +3549,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y261"/>
+  <dimension ref="A1:Y263"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R203" sqref="R203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3578,7 +3575,7 @@
     <col min="15" max="15" width="20.28515625" style="6" customWidth="1"/>
     <col min="16" max="16" width="18.7109375" style="6" customWidth="1"/>
     <col min="17" max="17" width="18.85546875" style="8" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="8" customWidth="1"/>
     <col min="19" max="19" width="20" style="8" customWidth="1"/>
     <col min="20" max="20" width="57.85546875" style="9" customWidth="1"/>
     <col min="21" max="21" width="53.140625" style="8" bestFit="1" customWidth="1"/>
@@ -3608,10 +3605,10 @@
         <v>106</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>343</v>
@@ -3643,7 +3640,7 @@
     </row>
     <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>186</v>
@@ -3693,7 +3690,7 @@
         <v>107</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>382</v>
@@ -3725,7 +3722,7 @@
         <v>303</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>382</v>
@@ -3810,7 +3807,7 @@
         <v>144</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>329</v>
@@ -3845,7 +3842,7 @@
         <v>109</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>331</v>
@@ -3895,7 +3892,7 @@
         <v>146</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>330</v>
@@ -4195,7 +4192,7 @@
         <v>92</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>451</v>
@@ -4242,7 +4239,7 @@
         <v>109</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>332</v>
@@ -4292,7 +4289,7 @@
         <v>174</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>334</v>
@@ -4339,7 +4336,7 @@
         <v>144</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q17" s="4" t="s">
         <v>131</v>
@@ -4386,7 +4383,7 @@
         <v>144</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>335</v>
@@ -4436,7 +4433,7 @@
         <v>109</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q19" s="8" t="s">
         <v>332</v>
@@ -4489,7 +4486,7 @@
         <v>144</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>336</v>
@@ -4631,7 +4628,7 @@
         <v>144</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>338</v>
@@ -4675,7 +4672,7 @@
         <v>109</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>195</v>
@@ -4722,7 +4719,7 @@
         <v>146</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>195</v>
@@ -4813,7 +4810,7 @@
         <v>144</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q27" s="4" t="s">
         <v>131</v>
@@ -4869,7 +4866,7 @@
         <v>144</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q28" s="4" t="s">
         <v>131</v>
@@ -4925,7 +4922,7 @@
         <v>144</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q29" s="4" t="s">
         <v>131</v>
@@ -4981,7 +4978,7 @@
         <v>109</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>332</v>
@@ -5040,7 +5037,7 @@
         <v>174</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>334</v>
@@ -5341,7 +5338,7 @@
         <v>92</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>451</v>
@@ -5491,7 +5488,7 @@
         <v>144</v>
       </c>
       <c r="P39" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q39" s="4" t="s">
         <v>131</v>
@@ -5550,7 +5547,7 @@
         <v>144</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q40" s="4" t="s">
         <v>131</v>
@@ -5667,7 +5664,7 @@
         <v>303</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>407</v>
@@ -5963,7 +5960,7 @@
         <v>92</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q49" s="3" t="s">
         <v>451</v>
@@ -6013,7 +6010,7 @@
         <v>109</v>
       </c>
       <c r="P50" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q50" s="8" t="s">
         <v>295</v>
@@ -6060,7 +6057,7 @@
         <v>174</v>
       </c>
       <c r="P51" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>334</v>
@@ -6106,7 +6103,7 @@
         <v>144</v>
       </c>
       <c r="P52" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q52" s="4" t="s">
         <v>131</v>
@@ -6156,7 +6153,7 @@
         <v>144</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q53" s="3" t="s">
         <v>335</v>
@@ -6209,7 +6206,7 @@
         <v>109</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q54" s="3" t="s">
         <v>332</v>
@@ -6265,7 +6262,7 @@
         <v>144</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>336</v>
@@ -6422,7 +6419,7 @@
         <v>144</v>
       </c>
       <c r="P58" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q58" s="4" t="s">
         <v>131</v>
@@ -6478,7 +6475,7 @@
         <v>109</v>
       </c>
       <c r="P59" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q59" s="4" t="s">
         <v>298</v>
@@ -6531,7 +6528,7 @@
         <v>146</v>
       </c>
       <c r="P60" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q60" s="4" t="s">
         <v>298</v>
@@ -6581,7 +6578,7 @@
         <v>144</v>
       </c>
       <c r="P61" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q61" s="4" t="s">
         <v>131</v>
@@ -6713,7 +6710,7 @@
         <v>144</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q64" s="4" t="s">
         <v>131</v>
@@ -6763,7 +6760,7 @@
         <v>144</v>
       </c>
       <c r="P65" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Q65" s="3" t="s">
         <v>350</v>
@@ -6945,7 +6942,7 @@
         <v>144</v>
       </c>
       <c r="P69" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q69" s="4" t="s">
         <v>131</v>
@@ -6989,7 +6986,7 @@
         <v>144</v>
       </c>
       <c r="P70" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q70" s="4" t="s">
         <v>131</v>
@@ -7036,7 +7033,7 @@
         <v>144</v>
       </c>
       <c r="P71" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q71" s="4" t="s">
         <v>131</v>
@@ -7086,7 +7083,7 @@
         <v>144</v>
       </c>
       <c r="P72" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="Q72" s="4" t="s">
         <v>131</v>
@@ -7321,7 +7318,7 @@
         <v>144</v>
       </c>
       <c r="P77" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q77" s="4" t="s">
         <v>131</v>
@@ -7377,7 +7374,7 @@
         <v>144</v>
       </c>
       <c r="P78" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q78" s="4" t="s">
         <v>131</v>
@@ -7430,7 +7427,7 @@
         <v>109</v>
       </c>
       <c r="P79" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q79" s="3" t="s">
         <v>295</v>
@@ -7480,7 +7477,7 @@
         <v>174</v>
       </c>
       <c r="P80" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q80" s="3" t="s">
         <v>295</v>
@@ -7775,7 +7772,7 @@
         <v>92</v>
       </c>
       <c r="P85" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q85" s="3" t="s">
         <v>451</v>
@@ -7828,7 +7825,7 @@
         <v>229</v>
       </c>
       <c r="P86" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q86" s="3" t="s">
         <v>381</v>
@@ -7843,7 +7840,7 @@
         <v>416</v>
       </c>
       <c r="U86" s="8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="X86" s="6" t="s">
         <v>399</v>
@@ -7878,7 +7875,7 @@
         <v>144</v>
       </c>
       <c r="P87" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q87" s="3" t="s">
         <v>401</v>
@@ -7905,7 +7902,7 @@
         <v>105</v>
       </c>
       <c r="Y87" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="88" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -7934,7 +7931,7 @@
         <v>144</v>
       </c>
       <c r="P88" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q88" s="4" t="s">
         <v>131</v>
@@ -7984,13 +7981,13 @@
         <v>131</v>
       </c>
       <c r="R89" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="S89" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T89" s="9" t="s">
         <v>513</v>
-      </c>
-      <c r="S89" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="T89" s="9" t="s">
-        <v>514</v>
       </c>
       <c r="X89" s="6" t="s">
         <v>119</v>
@@ -8119,7 +8116,7 @@
         <v>303</v>
       </c>
       <c r="P92" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q92" s="3" t="s">
         <v>409</v>
@@ -8225,7 +8222,7 @@
         <v>144</v>
       </c>
       <c r="P94" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q94" s="4" t="s">
         <v>131</v>
@@ -8284,7 +8281,7 @@
         <v>144</v>
       </c>
       <c r="P95" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q95" s="3" t="s">
         <v>413</v>
@@ -8613,7 +8610,7 @@
         <v>92</v>
       </c>
       <c r="P100" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q100" s="3" t="s">
         <v>451</v>
@@ -8784,7 +8781,7 @@
         <v>144</v>
       </c>
       <c r="P103" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q103" s="4" t="s">
         <v>131</v>
@@ -8846,7 +8843,7 @@
         <v>144</v>
       </c>
       <c r="P104" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Q104" s="3" t="s">
         <v>350</v>
@@ -9076,7 +9073,7 @@
         <v>144</v>
       </c>
       <c r="P108" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q108" s="4" t="s">
         <v>131</v>
@@ -9132,7 +9129,7 @@
         <v>144</v>
       </c>
       <c r="P109" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q109" s="4" t="s">
         <v>131</v>
@@ -9191,7 +9188,7 @@
         <v>144</v>
       </c>
       <c r="P110" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q110" s="4" t="s">
         <v>131</v>
@@ -9253,7 +9250,7 @@
         <v>144</v>
       </c>
       <c r="P111" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="Q111" s="4" t="s">
         <v>131</v>
@@ -9662,7 +9659,7 @@
         <v>92</v>
       </c>
       <c r="P119" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q119" s="3" t="s">
         <v>451</v>
@@ -9718,7 +9715,7 @@
         <v>109</v>
       </c>
       <c r="P120" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q120" s="8" t="s">
         <v>295</v>
@@ -9771,7 +9768,7 @@
         <v>174</v>
       </c>
       <c r="P121" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q121" s="3" t="s">
         <v>334</v>
@@ -9823,7 +9820,7 @@
         <v>144</v>
       </c>
       <c r="P122" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q122" s="4" t="s">
         <v>131</v>
@@ -9879,7 +9876,7 @@
         <v>144</v>
       </c>
       <c r="P123" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q123" s="3" t="s">
         <v>335</v>
@@ -9938,7 +9935,7 @@
         <v>109</v>
       </c>
       <c r="P124" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q124" s="3" t="s">
         <v>332</v>
@@ -10000,7 +9997,7 @@
         <v>144</v>
       </c>
       <c r="P125" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q125" s="3" t="s">
         <v>336</v>
@@ -10130,7 +10127,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="16" t="s">
         <v>179</v>
       </c>
@@ -10219,7 +10216,7 @@
         <v>109</v>
       </c>
       <c r="P129" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q129" s="4" t="s">
         <v>131</v>
@@ -10275,7 +10272,7 @@
         <v>146</v>
       </c>
       <c r="P130" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q130" s="4" t="s">
         <v>131</v>
@@ -10384,7 +10381,7 @@
         <v>144</v>
       </c>
       <c r="P132" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q132" s="4" t="s">
         <v>131</v>
@@ -10443,7 +10440,7 @@
         <v>144</v>
       </c>
       <c r="P133" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q133" s="4" t="s">
         <v>131</v>
@@ -10614,7 +10611,7 @@
         <v>144</v>
       </c>
       <c r="P136" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q136" s="4" t="s">
         <v>131</v>
@@ -10676,7 +10673,7 @@
         <v>109</v>
       </c>
       <c r="P137" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q137" s="4" t="s">
         <v>298</v>
@@ -10735,7 +10732,7 @@
         <v>146</v>
       </c>
       <c r="P138" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q138" s="4" t="s">
         <v>298</v>
@@ -10791,7 +10788,7 @@
         <v>144</v>
       </c>
       <c r="P139" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q139" s="4" t="s">
         <v>131</v>
@@ -10941,7 +10938,7 @@
         <v>144</v>
       </c>
       <c r="P142" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q142" s="4" t="s">
         <v>131</v>
@@ -10997,7 +10994,7 @@
         <v>144</v>
       </c>
       <c r="P143" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Q143" s="3" t="s">
         <v>350</v>
@@ -11203,7 +11200,7 @@
         <v>144</v>
       </c>
       <c r="P147" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q147" s="4" t="s">
         <v>131</v>
@@ -11253,7 +11250,7 @@
         <v>144</v>
       </c>
       <c r="P148" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q148" s="4" t="s">
         <v>131</v>
@@ -11362,7 +11359,7 @@
         <v>144</v>
       </c>
       <c r="P150" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="Q150" s="4" t="s">
         <v>131</v>
@@ -11627,7 +11624,7 @@
         <v>144</v>
       </c>
       <c r="P155" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q155" s="4" t="s">
         <v>131</v>
@@ -11689,7 +11686,7 @@
         <v>144</v>
       </c>
       <c r="P156" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q156" s="4" t="s">
         <v>131</v>
@@ -12015,7 +12012,7 @@
         <v>92</v>
       </c>
       <c r="P161" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q161" s="3" t="s">
         <v>451</v>
@@ -12074,7 +12071,7 @@
         <v>229</v>
       </c>
       <c r="P162" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q162" s="3" t="s">
         <v>381</v>
@@ -12089,7 +12086,7 @@
         <v>416</v>
       </c>
       <c r="U162" s="8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="X162" s="6" t="s">
         <v>399</v>
@@ -12130,7 +12127,7 @@
         <v>144</v>
       </c>
       <c r="P163" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q163" s="3" t="s">
         <v>401</v>
@@ -12157,7 +12154,7 @@
         <v>105</v>
       </c>
       <c r="Y163" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="164" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -12192,7 +12189,7 @@
         <v>144</v>
       </c>
       <c r="P164" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q164" s="4" t="s">
         <v>131</v>
@@ -12248,13 +12245,13 @@
         <v>131</v>
       </c>
       <c r="R165" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="S165" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T165" s="9" t="s">
         <v>513</v>
-      </c>
-      <c r="S165" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="T165" s="9" t="s">
-        <v>514</v>
       </c>
       <c r="X165" s="6" t="s">
         <v>119</v>
@@ -12401,7 +12398,7 @@
         <v>303</v>
       </c>
       <c r="P168" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q168" s="3" t="s">
         <v>409</v>
@@ -12519,7 +12516,7 @@
         <v>144</v>
       </c>
       <c r="P170" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q170" s="4" t="s">
         <v>131</v>
@@ -12584,7 +12581,7 @@
         <v>144</v>
       </c>
       <c r="P171" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q171" s="3" t="s">
         <v>332</v>
@@ -12938,7 +12935,7 @@
         <v>92</v>
       </c>
       <c r="P176" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q176" s="3" t="s">
         <v>451</v>
@@ -13127,7 +13124,7 @@
         <v>144</v>
       </c>
       <c r="P179" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q179" s="4" t="s">
         <v>131</v>
@@ -13453,7 +13450,7 @@
         <v>144</v>
       </c>
       <c r="P184" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q184" s="4" t="s">
         <v>131</v>
@@ -13521,7 +13518,7 @@
         <v>144</v>
       </c>
       <c r="P185" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q185" s="4" t="s">
         <v>131</v>
@@ -13586,7 +13583,7 @@
         <v>144</v>
       </c>
       <c r="P186" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q186" s="4" t="s">
         <v>131</v>
@@ -13654,7 +13651,7 @@
         <v>144</v>
       </c>
       <c r="P187" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="Q187" s="4" t="s">
         <v>131</v>
@@ -13710,10 +13707,10 @@
         <v>371</v>
       </c>
       <c r="V188" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="W188" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="X188" s="6" t="s">
         <v>119</v>
@@ -13748,7 +13745,7 @@
         <v>377</v>
       </c>
       <c r="T189" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="X189" s="6" t="s">
         <v>119</v>
@@ -13786,16 +13783,16 @@
         <v>381</v>
       </c>
       <c r="T190" s="9" t="s">
-        <v>459</v>
+        <v>384</v>
       </c>
       <c r="U190" s="8" t="s">
         <v>385</v>
       </c>
       <c r="V190" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="W190" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="X190" s="6" t="s">
         <v>119</v>
@@ -13862,7 +13859,7 @@
         <v>144</v>
       </c>
       <c r="P192" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q192" s="4" t="s">
         <v>131</v>
@@ -13912,7 +13909,7 @@
         <v>144</v>
       </c>
       <c r="P193" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q193" s="4" t="s">
         <v>131</v>
@@ -13959,7 +13956,7 @@
         <v>109</v>
       </c>
       <c r="P194" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q194" s="3" t="s">
         <v>295</v>
@@ -14003,7 +14000,7 @@
         <v>174</v>
       </c>
       <c r="P195" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q195" s="3" t="s">
         <v>295</v>
@@ -14268,7 +14265,7 @@
         <v>92</v>
       </c>
       <c r="P200" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q200" s="3" t="s">
         <v>451</v>
@@ -14315,7 +14312,7 @@
         <v>229</v>
       </c>
       <c r="P201" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q201" s="3" t="s">
         <v>381</v>
@@ -14330,7 +14327,7 @@
         <v>416</v>
       </c>
       <c r="U201" s="8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="X201" s="6" t="s">
         <v>399</v>
@@ -14359,7 +14356,7 @@
         <v>144</v>
       </c>
       <c r="P202" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q202" s="3" t="s">
         <v>401</v>
@@ -14386,7 +14383,7 @@
         <v>105</v>
       </c>
       <c r="Y202" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="203" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -14400,28 +14397,28 @@
         <v>378</v>
       </c>
       <c r="D203" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="N203" s="7" t="s">
-        <v>225</v>
+        <v>404</v>
+      </c>
+      <c r="N203" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="O203" s="6" t="s">
-        <v>229</v>
+        <v>144</v>
       </c>
       <c r="P203" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q203" s="3" t="s">
-        <v>381</v>
+        <v>498</v>
+      </c>
+      <c r="Q203" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="R203" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="S203" s="3" t="s">
-        <v>381</v>
+        <v>408</v>
+      </c>
+      <c r="S203" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="T203" s="9" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="X203" s="6" t="s">
         <v>119</v>
@@ -14438,31 +14435,28 @@
         <v>378</v>
       </c>
       <c r="D204" s="15" t="s">
-        <v>223</v>
+        <v>404</v>
       </c>
       <c r="E204" s="15" t="s">
-        <v>227</v>
+        <v>397</v>
       </c>
       <c r="N204" s="7" t="s">
         <v>131</v>
       </c>
       <c r="O204" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="P204" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q204" s="3" t="s">
-        <v>342</v>
+        <v>144</v>
+      </c>
+      <c r="Q204" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="R204" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="S204" s="3" t="s">
-        <v>342</v>
+        <v>512</v>
+      </c>
+      <c r="S204" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="T204" s="9" t="s">
-        <v>421</v>
+        <v>513</v>
       </c>
       <c r="X204" s="6" t="s">
         <v>119</v>
@@ -14481,41 +14475,32 @@
       <c r="D205" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="E205" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="F205" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="N205" s="6" t="s">
-        <v>304</v>
+      <c r="N205" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="O205" s="6" t="s">
-        <v>303</v>
+        <v>229</v>
       </c>
       <c r="P205" s="6" t="s">
-        <v>496</v>
+        <v>265</v>
       </c>
       <c r="Q205" s="3" t="s">
-        <v>409</v>
+        <v>381</v>
       </c>
       <c r="R205" s="3" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="S205" s="3" t="s">
-        <v>409</v>
+        <v>381</v>
       </c>
       <c r="T205" s="9" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="X205" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="Y205" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="206" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A206" s="16" t="s">
         <v>179</v>
       </c>
@@ -14529,13 +14514,10 @@
         <v>223</v>
       </c>
       <c r="E206" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="F206" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="N206" s="6" t="s">
-        <v>109</v>
+        <v>227</v>
+      </c>
+      <c r="N206" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="O206" s="6" t="s">
         <v>109</v>
@@ -14544,22 +14526,22 @@
         <v>265</v>
       </c>
       <c r="Q206" s="3" t="s">
-        <v>413</v>
+        <v>342</v>
       </c>
       <c r="R206" s="3" t="s">
-        <v>388</v>
+        <v>342</v>
       </c>
       <c r="S206" s="3" t="s">
-        <v>388</v>
+        <v>342</v>
       </c>
       <c r="T206" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="X206" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="X206" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="207" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="16" t="s">
         <v>179</v>
       </c>
@@ -14576,40 +14558,34 @@
         <v>230</v>
       </c>
       <c r="F207" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="G207" s="15" t="s">
-        <v>147</v>
+        <v>232</v>
       </c>
       <c r="N207" s="6" t="s">
-        <v>108</v>
+        <v>304</v>
       </c>
       <c r="O207" s="6" t="s">
-        <v>144</v>
+        <v>303</v>
       </c>
       <c r="P207" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q207" s="4" t="s">
-        <v>131</v>
+        <v>495</v>
+      </c>
+      <c r="Q207" s="3" t="s">
+        <v>409</v>
       </c>
       <c r="R207" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="S207" s="4" t="s">
-        <v>131</v>
+        <v>409</v>
+      </c>
+      <c r="S207" s="3" t="s">
+        <v>409</v>
       </c>
       <c r="T207" s="9" t="s">
-        <v>412</v>
-      </c>
-      <c r="W207" s="8" t="s">
-        <v>148</v>
+        <v>410</v>
       </c>
       <c r="X207" s="6" t="s">
         <v>119</v>
       </c>
       <c r="Y207" s="3" t="s">
-        <v>200</v>
+        <v>411</v>
       </c>
     </row>
     <row r="208" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -14631,44 +14607,32 @@
       <c r="F208" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G208" s="15" t="s">
-        <v>141</v>
-      </c>
       <c r="N208" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O208" s="6" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="P208" s="6" t="s">
-        <v>500</v>
+        <v>265</v>
       </c>
       <c r="Q208" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="R208" s="4" t="s">
-        <v>131</v>
+        <v>413</v>
+      </c>
+      <c r="R208" s="3" t="s">
+        <v>388</v>
       </c>
       <c r="S208" s="3" t="s">
-        <v>332</v>
+        <v>388</v>
       </c>
       <c r="T208" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="U208" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="V208" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="X208" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="X208" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="Y208" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="209" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="16" t="s">
         <v>179</v>
       </c>
@@ -14688,43 +14652,40 @@
         <v>113</v>
       </c>
       <c r="G209" s="15" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="N209" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O209" s="6" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="P209" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q209" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q209" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="R209" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="R209" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="S209" s="4" t="s">
         <v>131</v>
       </c>
       <c r="T209" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="U209" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="V209" s="8" t="s">
-        <v>132</v>
+        <v>412</v>
       </c>
       <c r="W209" s="8" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="X209" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="210" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="Y209" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="210" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="16" t="s">
         <v>179</v>
       </c>
@@ -14744,47 +14705,43 @@
         <v>113</v>
       </c>
       <c r="G210" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="H210" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="I210" s="17"/>
-      <c r="L210" s="17"/>
-      <c r="M210" s="17"/>
+        <v>141</v>
+      </c>
       <c r="N210" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="O210" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="P210" s="7"/>
+        <v>108</v>
+      </c>
+      <c r="O210" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="P210" s="6" t="s">
+        <v>499</v>
+      </c>
       <c r="Q210" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R210" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="S210" s="4" t="s">
-        <v>131</v>
+      <c r="S210" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="T210" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="U210" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="V210" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="W210" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="X210" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="U210" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="V210" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="X210" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y210" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="211" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A211" s="16" t="s">
         <v>179</v>
       </c>
@@ -14806,11 +14763,8 @@
       <c r="G211" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="H211" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="N211" s="7" t="s">
-        <v>131</v>
+      <c r="N211" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O211" s="6" t="s">
         <v>109</v>
@@ -14819,7 +14773,7 @@
         <v>265</v>
       </c>
       <c r="Q211" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R211" s="4" t="s">
         <v>131</v>
@@ -14828,22 +14782,22 @@
         <v>131</v>
       </c>
       <c r="T211" s="9" t="s">
-        <v>420</v>
+        <v>285</v>
       </c>
       <c r="U211" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="V211" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="W211" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="X211" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V211" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="W211" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="X211" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="212" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A212" s="16" t="s">
         <v>179</v>
       </c>
@@ -14865,23 +14819,21 @@
       <c r="G212" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="H212" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="I212" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="N212" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="O212" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="P212" s="6" t="s">
-        <v>380</v>
-      </c>
+      <c r="H212" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I212" s="17"/>
+      <c r="L212" s="17"/>
+      <c r="M212" s="17"/>
+      <c r="N212" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="O212" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="P212" s="7"/>
       <c r="Q212" s="3" t="s">
-        <v>451</v>
+        <v>333</v>
       </c>
       <c r="R212" s="4" t="s">
         <v>131</v>
@@ -14890,7 +14842,7 @@
         <v>131</v>
       </c>
       <c r="T212" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="U212" s="10" t="s">
         <v>105</v>
@@ -14905,7 +14857,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="213" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A213" s="16" t="s">
         <v>179</v>
       </c>
@@ -14930,20 +14882,17 @@
       <c r="H213" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="I213" s="15" t="s">
-        <v>139</v>
-      </c>
       <c r="N213" s="7" t="s">
         <v>131</v>
       </c>
       <c r="O213" s="6" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="P213" s="6" t="s">
-        <v>504</v>
+        <v>265</v>
       </c>
       <c r="Q213" s="3" t="s">
-        <v>451</v>
+        <v>333</v>
       </c>
       <c r="R213" s="4" t="s">
         <v>131</v>
@@ -14952,7 +14901,7 @@
         <v>131</v>
       </c>
       <c r="T213" s="9" t="s">
-        <v>140</v>
+        <v>420</v>
       </c>
       <c r="U213" s="10" t="s">
         <v>105</v>
@@ -14967,7 +14916,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="214" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A214" s="16" t="s">
         <v>179</v>
       </c>
@@ -14984,34 +14933,52 @@
         <v>230</v>
       </c>
       <c r="F214" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="N214" s="6" t="s">
-        <v>302</v>
+        <v>113</v>
+      </c>
+      <c r="G214" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H214" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I214" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="N214" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="O214" s="6" t="s">
-        <v>229</v>
+        <v>92</v>
       </c>
       <c r="P214" s="6" t="s">
-        <v>265</v>
+        <v>380</v>
       </c>
       <c r="Q214" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="R214" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="S214" s="3" t="s">
-        <v>346</v>
+        <v>451</v>
+      </c>
+      <c r="R214" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S214" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="T214" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="X214" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="215" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="U214" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="V214" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="W214" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="X214" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="215" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="16" t="s">
         <v>179</v>
       </c>
@@ -15028,34 +14995,49 @@
         <v>230</v>
       </c>
       <c r="F215" s="15" t="s">
-        <v>301</v>
+        <v>113</v>
       </c>
       <c r="G215" s="15" t="s">
-        <v>305</v>
+        <v>125</v>
+      </c>
+      <c r="H215" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I215" s="15" t="s">
+        <v>139</v>
       </c>
       <c r="N215" s="7" t="s">
         <v>131</v>
       </c>
       <c r="O215" s="6" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="P215" s="6" t="s">
-        <v>265</v>
+        <v>503</v>
       </c>
       <c r="Q215" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="R215" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="S215" s="3" t="s">
-        <v>348</v>
+        <v>451</v>
+      </c>
+      <c r="R215" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S215" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="T215" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="X215" s="6" t="s">
-        <v>119</v>
+        <v>140</v>
+      </c>
+      <c r="U215" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="V215" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="W215" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="X215" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="216" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -15077,47 +15059,32 @@
       <c r="F216" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="G216" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="H216" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="I216" s="15" t="s">
-        <v>141</v>
-      </c>
       <c r="N216" s="6" t="s">
-        <v>108</v>
+        <v>302</v>
       </c>
       <c r="O216" s="6" t="s">
-        <v>144</v>
+        <v>229</v>
       </c>
       <c r="P216" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q216" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="R216" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="S216" s="8" t="s">
-        <v>349</v>
+        <v>265</v>
+      </c>
+      <c r="Q216" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="R216" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="S216" s="3" t="s">
+        <v>346</v>
       </c>
       <c r="T216" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="W216" s="8" t="s">
-        <v>311</v>
+        <v>415</v>
       </c>
       <c r="X216" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="Y216" s="3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="217" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="16" t="s">
         <v>179</v>
       </c>
@@ -15137,46 +15104,34 @@
         <v>301</v>
       </c>
       <c r="G217" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="H217" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="N217" s="6" t="s">
-        <v>108</v>
+        <v>305</v>
+      </c>
+      <c r="N217" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="O217" s="6" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="P217" s="6" t="s">
-        <v>508</v>
+        <v>265</v>
       </c>
       <c r="Q217" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="R217" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="S217" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="T217" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="U217" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="V217" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="W217" s="8" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="X217" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="218" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A218" s="16" t="s">
         <v>179</v>
       </c>
@@ -15193,35 +15148,49 @@
         <v>230</v>
       </c>
       <c r="F218" s="15" t="s">
-        <v>314</v>
+        <v>301</v>
+      </c>
+      <c r="G218" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="H218" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I218" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="N218" s="6" t="s">
-        <v>315</v>
+        <v>108</v>
       </c>
       <c r="O218" s="6" t="s">
-        <v>229</v>
+        <v>144</v>
       </c>
       <c r="P218" s="6" t="s">
-        <v>265</v>
+        <v>499</v>
       </c>
       <c r="Q218" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="R218" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="S218" s="3" t="s">
-        <v>351</v>
+      <c r="R218" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S218" s="8" t="s">
+        <v>349</v>
       </c>
       <c r="T218" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="W218" s="3"/>
+        <v>312</v>
+      </c>
+      <c r="W218" s="8" t="s">
+        <v>311</v>
+      </c>
       <c r="X218" s="6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y218" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="219" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="16" t="s">
         <v>179</v>
       </c>
@@ -15238,31 +15207,43 @@
         <v>230</v>
       </c>
       <c r="F219" s="15" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="G219" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="N219" s="7" t="s">
-        <v>131</v>
+        <v>306</v>
+      </c>
+      <c r="H219" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="N219" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="O219" s="6" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="P219" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q219" s="4" t="s">
-        <v>131</v>
+        <v>507</v>
+      </c>
+      <c r="Q219" s="3" t="s">
+        <v>350</v>
       </c>
       <c r="R219" s="3" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
       <c r="S219" s="3" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
       <c r="T219" s="9" t="s">
-        <v>317</v>
+        <v>308</v>
+      </c>
+      <c r="U219" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="V219" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="W219" s="8" t="s">
+        <v>310</v>
       </c>
       <c r="X219" s="6" t="s">
         <v>119</v>
@@ -15287,17 +15268,11 @@
       <c r="F220" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="G220" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="H220" s="15" t="s">
-        <v>113</v>
-      </c>
       <c r="N220" s="6" t="s">
-        <v>109</v>
+        <v>315</v>
       </c>
       <c r="O220" s="6" t="s">
-        <v>109</v>
+        <v>229</v>
       </c>
       <c r="P220" s="6" t="s">
         <v>265</v>
@@ -15306,22 +15281,20 @@
         <v>131</v>
       </c>
       <c r="R220" s="3" t="s">
-        <v>455</v>
+        <v>351</v>
       </c>
       <c r="S220" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="T220" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="V220" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="X220" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="W220" s="3"/>
+      <c r="X220" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="221" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A221" s="16" t="s">
         <v>179</v>
       </c>
@@ -15341,37 +15314,28 @@
         <v>314</v>
       </c>
       <c r="G221" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="H221" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="I221" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="N221" s="6" t="s">
-        <v>108</v>
+        <v>316</v>
+      </c>
+      <c r="N221" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="O221" s="6" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="P221" s="6" t="s">
-        <v>500</v>
+        <v>265</v>
       </c>
       <c r="Q221" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="R221" s="4" t="s">
-        <v>131</v>
+      <c r="R221" s="3" t="s">
+        <v>376</v>
       </c>
       <c r="S221" s="3" t="s">
-        <v>352</v>
+        <v>376</v>
       </c>
       <c r="T221" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="W221" s="8" t="s">
-        <v>148</v>
+        <v>317</v>
       </c>
       <c r="X221" s="6" t="s">
         <v>119</v>
@@ -15402,38 +15366,35 @@
       <c r="H222" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="I222" s="15" t="s">
-        <v>141</v>
-      </c>
       <c r="N222" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O222" s="6" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="P222" s="6" t="s">
-        <v>500</v>
+        <v>265</v>
       </c>
       <c r="Q222" s="4" t="s">
         <v>131</v>
       </c>
       <c r="R222" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="S222" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="S222" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="T222" s="9" t="s">
-        <v>326</v>
+        <v>422</v>
       </c>
       <c r="V222" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="X222" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="X222" s="13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="223" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="16" t="s">
         <v>179</v>
       </c>
@@ -15456,7 +15417,10 @@
         <v>318</v>
       </c>
       <c r="H223" s="15" t="s">
-        <v>319</v>
+        <v>113</v>
+      </c>
+      <c r="I223" s="15" t="s">
+        <v>147</v>
       </c>
       <c r="N223" s="6" t="s">
         <v>108</v>
@@ -15470,26 +15434,23 @@
       <c r="Q223" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="R223" s="3" t="s">
-        <v>353</v>
+      <c r="R223" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="S223" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T223" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="V223" s="8" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="W223" s="8" t="s">
-        <v>323</v>
+        <v>148</v>
       </c>
       <c r="X223" s="6" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="224" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="224" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="16" t="s">
         <v>179</v>
       </c>
@@ -15512,7 +15473,10 @@
         <v>318</v>
       </c>
       <c r="H224" s="15" t="s">
-        <v>324</v>
+        <v>113</v>
+      </c>
+      <c r="I224" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="N224" s="6" t="s">
         <v>108</v>
@@ -15521,181 +15485,211 @@
         <v>144</v>
       </c>
       <c r="P224" s="6" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="Q224" s="4" t="s">
         <v>131</v>
       </c>
       <c r="R224" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="S224" s="3" t="s">
         <v>352</v>
       </c>
+      <c r="S224" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="T224" s="9" t="s">
-        <v>354</v>
+        <v>326</v>
       </c>
       <c r="V224" s="8" t="s">
-        <v>423</v>
+        <v>327</v>
       </c>
       <c r="X224" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="Y224" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="225" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="225" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A225" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B225" s="15" t="s">
-        <v>463</v>
-      </c>
-      <c r="N225" s="7" t="s">
-        <v>224</v>
+        <v>356</v>
+      </c>
+      <c r="C225" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D225" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="E225" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="F225" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="G225" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="H225" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="N225" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="O225" s="6" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="P225" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q225" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="R225" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="S225" s="4" t="s">
-        <v>131</v>
+        <v>498</v>
+      </c>
+      <c r="Q225" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="R225" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="S225" s="3" t="s">
+        <v>353</v>
       </c>
       <c r="T225" s="9" t="s">
-        <v>465</v>
-      </c>
-      <c r="U225" s="8" t="s">
-        <v>468</v>
+        <v>322</v>
+      </c>
+      <c r="V225" s="8" t="s">
+        <v>321</v>
       </c>
       <c r="W225" s="8" t="s">
-        <v>467</v>
+        <v>323</v>
       </c>
       <c r="X225" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="226" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A226" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B226" s="15" t="s">
-        <v>463</v>
+        <v>356</v>
       </c>
       <c r="C226" s="15" t="s">
-        <v>103</v>
+        <v>378</v>
+      </c>
+      <c r="D226" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="E226" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="F226" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="G226" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="H226" s="15" t="s">
+        <v>324</v>
       </c>
       <c r="N226" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O226" s="6" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="P226" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q226" s="3" t="s">
-        <v>464</v>
+        <v>502</v>
+      </c>
+      <c r="Q226" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="R226" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="S226" s="4" t="s">
-        <v>131</v>
+        <v>424</v>
+      </c>
+      <c r="S226" s="3" t="s">
+        <v>352</v>
       </c>
       <c r="T226" s="9" t="s">
-        <v>466</v>
-      </c>
-      <c r="U226" s="10"/>
-      <c r="V226" s="10"/>
-      <c r="W226" s="10"/>
+        <v>354</v>
+      </c>
+      <c r="V226" s="8" t="s">
+        <v>423</v>
+      </c>
       <c r="X226" s="6" t="s">
         <v>119</v>
       </c>
+      <c r="Y226" s="3" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="227" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B227" s="15" t="s">
-        <v>463</v>
-      </c>
-      <c r="C227" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D227" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="N227" s="6" t="s">
-        <v>108</v>
+        <v>462</v>
+      </c>
+      <c r="N227" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="O227" s="6" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="P227" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="Q227" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="R227" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="S227" s="3" t="s">
-        <v>338</v>
+        <v>265</v>
+      </c>
+      <c r="Q227" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="R227" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="S227" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="T227" s="9" t="s">
-        <v>469</v>
+        <v>464</v>
+      </c>
+      <c r="U227" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="W227" s="8" t="s">
+        <v>466</v>
       </c>
       <c r="X227" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="228" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A228" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B228" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C228" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D228" s="15" t="s">
-        <v>115</v>
-      </c>
       <c r="N228" s="6" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="O228" s="6" t="s">
         <v>109</v>
       </c>
       <c r="P228" s="6" t="s">
-        <v>498</v>
+        <v>265</v>
       </c>
       <c r="Q228" s="3" t="s">
-        <v>195</v>
+        <v>463</v>
       </c>
       <c r="R228" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="S228" s="3" t="s">
-        <v>331</v>
+        <v>463</v>
+      </c>
+      <c r="S228" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="T228" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="U228" s="8" t="s">
-        <v>471</v>
-      </c>
+        <v>465</v>
+      </c>
+      <c r="U228" s="10"/>
+      <c r="V228" s="10"/>
+      <c r="W228" s="10"/>
       <c r="X228" s="6" t="s">
         <v>119</v>
       </c>
@@ -15705,69 +15699,63 @@
         <v>179</v>
       </c>
       <c r="B229" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C229" s="15" t="s">
         <v>103</v>
       </c>
       <c r="D229" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="E229" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="N229" s="7" t="s">
-        <v>131</v>
+        <v>110</v>
+      </c>
+      <c r="N229" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="O229" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P229" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="Q229" s="3" t="s">
-        <v>195</v>
+        <v>338</v>
       </c>
       <c r="R229" s="3" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="S229" s="3" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="T229" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="U229" s="10" t="s">
-        <v>105</v>
+        <v>468</v>
       </c>
       <c r="X229" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B230" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C230" s="15" t="s">
         <v>103</v>
       </c>
       <c r="D230" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="N230" s="6" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="O230" s="6" t="s">
         <v>109</v>
       </c>
       <c r="P230" s="6" t="s">
-        <v>265</v>
+        <v>497</v>
       </c>
       <c r="Q230" s="3" t="s">
-        <v>331</v>
+        <v>195</v>
       </c>
       <c r="R230" s="3" t="s">
         <v>331</v>
@@ -15776,9 +15764,12 @@
         <v>331</v>
       </c>
       <c r="T230" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="X230" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="U230" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="X230" s="6" t="s">
         <v>119</v>
       </c>
     </row>
@@ -15787,57 +15778,51 @@
         <v>179</v>
       </c>
       <c r="B231" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C231" s="15" t="s">
         <v>103</v>
       </c>
       <c r="D231" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E231" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="N231" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
+      </c>
+      <c r="N231" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="O231" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="P231" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q231" s="4" t="s">
-        <v>131</v>
+        <v>497</v>
+      </c>
+      <c r="Q231" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="R231" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="S231" s="4" t="s">
-        <v>131</v>
+        <v>330</v>
+      </c>
+      <c r="S231" s="3" t="s">
+        <v>330</v>
       </c>
       <c r="T231" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="U231" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="W231" s="8" t="s">
-        <v>148</v>
+        <v>471</v>
+      </c>
+      <c r="U231" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="X231" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="Y231" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="232" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A232" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B232" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C232" s="15" t="s">
         <v>103</v>
@@ -15845,41 +15830,29 @@
       <c r="D232" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="E232" s="15" t="s">
-        <v>147</v>
-      </c>
       <c r="N232" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O232" s="6" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="P232" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q232" s="4" t="s">
-        <v>131</v>
+        <v>265</v>
+      </c>
+      <c r="Q232" s="3" t="s">
+        <v>331</v>
       </c>
       <c r="R232" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="S232" s="4" t="s">
-        <v>131</v>
+        <v>331</v>
+      </c>
+      <c r="S232" s="3" t="s">
+        <v>331</v>
       </c>
       <c r="T232" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="U232" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="W232" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="X232" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="X232" s="13" t="s">
         <v>119</v>
-      </c>
-      <c r="Y232" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="233" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -15887,7 +15860,7 @@
         <v>179</v>
       </c>
       <c r="B233" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C233" s="15" t="s">
         <v>103</v>
@@ -15896,7 +15869,7 @@
         <v>113</v>
       </c>
       <c r="E233" s="15" t="s">
-        <v>141</v>
+        <v>201</v>
       </c>
       <c r="N233" s="6" t="s">
         <v>108</v>
@@ -15905,25 +15878,25 @@
         <v>144</v>
       </c>
       <c r="P233" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q233" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="R233" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="S233" s="3" t="s">
+      <c r="R233" s="3" t="s">
         <v>332</v>
       </c>
+      <c r="S233" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="T233" s="9" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="U233" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="V233" s="8" t="s">
-        <v>199</v>
+        <v>205</v>
+      </c>
+      <c r="W233" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="X233" s="6" t="s">
         <v>119</v>
@@ -15932,12 +15905,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="234" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B234" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C234" s="15" t="s">
         <v>103</v>
@@ -15946,40 +15919,40 @@
         <v>113</v>
       </c>
       <c r="E234" s="15" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="N234" s="6" t="s">
-        <v>167</v>
+        <v>108</v>
       </c>
       <c r="O234" s="6" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="P234" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="Q234" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q234" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="R234" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="R234" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="S234" s="4" t="s">
         <v>131</v>
       </c>
       <c r="T234" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="U234" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="V234" s="8" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="W234" s="8" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="X234" s="6" t="s">
-        <v>168</v>
+        <v>119</v>
+      </c>
+      <c r="Y234" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="235" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -15987,7 +15960,7 @@
         <v>179</v>
       </c>
       <c r="B235" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C235" s="15" t="s">
         <v>103</v>
@@ -15996,51 +15969,48 @@
         <v>113</v>
       </c>
       <c r="E235" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="F235" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="N235" s="7" t="s">
-        <v>131</v>
+        <v>141</v>
+      </c>
+      <c r="N235" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="O235" s="6" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="P235" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="Q235" s="3" t="s">
-        <v>334</v>
+        <v>499</v>
+      </c>
+      <c r="Q235" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="R235" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="S235" s="4" t="s">
-        <v>131</v>
+      <c r="S235" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="T235" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="U235" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="V235" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="W235" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="X235" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="236" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="U235" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="V235" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="X235" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y235" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="236" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B236" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C236" s="15" t="s">
         <v>103</v>
@@ -16049,16 +16019,16 @@
         <v>113</v>
       </c>
       <c r="E236" s="15" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="N236" s="6" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="O236" s="6" t="s">
         <v>109</v>
       </c>
       <c r="P236" s="6" t="s">
-        <v>265</v>
+        <v>495</v>
       </c>
       <c r="Q236" s="3" t="s">
         <v>332</v>
@@ -16070,10 +16040,10 @@
         <v>131</v>
       </c>
       <c r="T236" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="U236" s="10" t="s">
-        <v>105</v>
+        <v>208</v>
+      </c>
+      <c r="U236" s="8" t="s">
+        <v>207</v>
       </c>
       <c r="V236" s="8" t="s">
         <v>132</v>
@@ -16082,15 +16052,15 @@
         <v>133</v>
       </c>
       <c r="X236" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="237" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="237" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B237" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C237" s="15" t="s">
         <v>103</v>
@@ -16099,25 +16069,22 @@
         <v>113</v>
       </c>
       <c r="E237" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="F237" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G237" s="17"/>
-      <c r="J237" s="17"/>
-      <c r="K237" s="17"/>
-      <c r="L237" s="17"/>
-      <c r="M237" s="17"/>
-      <c r="N237" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="O237" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="P237" s="7"/>
+        <v>162</v>
+      </c>
+      <c r="F237" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="N237" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="O237" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="P237" s="6" t="s">
+        <v>495</v>
+      </c>
       <c r="Q237" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="R237" s="4" t="s">
         <v>131</v>
@@ -16126,7 +16093,7 @@
         <v>131</v>
       </c>
       <c r="T237" s="9" t="s">
-        <v>134</v>
+        <v>209</v>
       </c>
       <c r="U237" s="10" t="s">
         <v>105</v>
@@ -16141,12 +16108,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="238" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" ht="90" x14ac:dyDescent="0.25">
       <c r="A238" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B238" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C238" s="15" t="s">
         <v>103</v>
@@ -16157,11 +16124,8 @@
       <c r="E238" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F238" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="N238" s="7" t="s">
-        <v>131</v>
+      <c r="N238" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O238" s="6" t="s">
         <v>109</v>
@@ -16170,7 +16134,7 @@
         <v>265</v>
       </c>
       <c r="Q238" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R238" s="4" t="s">
         <v>131</v>
@@ -16179,27 +16143,27 @@
         <v>131</v>
       </c>
       <c r="T238" s="9" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="U238" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="V238" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="W238" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="X238" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="239" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V238" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="W238" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="X238" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="239" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B239" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C239" s="15" t="s">
         <v>103</v>
@@ -16210,23 +16174,23 @@
       <c r="E239" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F239" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="G239" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="N239" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="O239" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="P239" s="6" t="s">
-        <v>380</v>
-      </c>
+      <c r="F239" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G239" s="17"/>
+      <c r="J239" s="17"/>
+      <c r="K239" s="17"/>
+      <c r="L239" s="17"/>
+      <c r="M239" s="17"/>
+      <c r="N239" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="O239" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="P239" s="7"/>
       <c r="Q239" s="3" t="s">
-        <v>451</v>
+        <v>333</v>
       </c>
       <c r="R239" s="4" t="s">
         <v>131</v>
@@ -16235,7 +16199,7 @@
         <v>131</v>
       </c>
       <c r="T239" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="U239" s="10" t="s">
         <v>105</v>
@@ -16250,12 +16214,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="240" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A240" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B240" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C240" s="15" t="s">
         <v>103</v>
@@ -16269,20 +16233,17 @@
       <c r="F240" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="G240" s="15" t="s">
-        <v>139</v>
-      </c>
       <c r="N240" s="7" t="s">
         <v>131</v>
       </c>
       <c r="O240" s="6" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="P240" s="6" t="s">
-        <v>504</v>
+        <v>265</v>
       </c>
       <c r="Q240" s="3" t="s">
-        <v>451</v>
+        <v>333</v>
       </c>
       <c r="R240" s="4" t="s">
         <v>131</v>
@@ -16291,7 +16252,7 @@
         <v>131</v>
       </c>
       <c r="T240" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="U240" s="10" t="s">
         <v>105</v>
@@ -16306,12 +16267,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="241" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A241" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B241" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C241" s="15" t="s">
         <v>103</v>
@@ -16320,19 +16281,25 @@
         <v>113</v>
       </c>
       <c r="E241" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="N241" s="6" t="s">
-        <v>170</v>
+        <v>125</v>
+      </c>
+      <c r="F241" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G241" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="N241" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="O241" s="6" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="P241" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="Q241" s="8" t="s">
-        <v>332</v>
+        <v>380</v>
+      </c>
+      <c r="Q241" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="R241" s="4" t="s">
         <v>131</v>
@@ -16341,10 +16308,10 @@
         <v>131</v>
       </c>
       <c r="T241" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="U241" s="11" t="s">
-        <v>176</v>
+        <v>138</v>
+      </c>
+      <c r="U241" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="V241" s="10" t="s">
         <v>105</v>
@@ -16352,16 +16319,16 @@
       <c r="W241" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="X241" s="13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X241" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="242" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B242" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C242" s="15" t="s">
         <v>103</v>
@@ -16370,25 +16337,25 @@
         <v>113</v>
       </c>
       <c r="E242" s="15" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="F242" s="15" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="G242" s="15" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="N242" s="7" t="s">
         <v>131</v>
       </c>
       <c r="O242" s="6" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="P242" s="6" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="Q242" s="3" t="s">
-        <v>336</v>
+        <v>451</v>
       </c>
       <c r="R242" s="4" t="s">
         <v>131</v>
@@ -16397,11 +16364,17 @@
         <v>131</v>
       </c>
       <c r="T242" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="U242" s="10"/>
-      <c r="V242" s="10"/>
-      <c r="W242" s="10"/>
+        <v>140</v>
+      </c>
+      <c r="U242" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="V242" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="W242" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="X242" s="12" t="s">
         <v>105</v>
       </c>
@@ -16411,7 +16384,7 @@
         <v>179</v>
       </c>
       <c r="B243" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C243" s="15" t="s">
         <v>103</v>
@@ -16420,16 +16393,16 @@
         <v>113</v>
       </c>
       <c r="E243" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="N243" s="7" t="s">
-        <v>224</v>
+        <v>169</v>
+      </c>
+      <c r="N243" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="O243" s="6" t="s">
         <v>109</v>
       </c>
       <c r="P243" s="6" t="s">
-        <v>265</v>
+        <v>498</v>
       </c>
       <c r="Q243" s="8" t="s">
         <v>332</v>
@@ -16441,21 +16414,27 @@
         <v>131</v>
       </c>
       <c r="T243" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="U243" s="8" t="s">
-        <v>476</v>
-      </c>
-      <c r="X243" s="6" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="U243" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="V243" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="W243" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="X243" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="244" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B244" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C244" s="15" t="s">
         <v>103</v>
@@ -16464,22 +16443,25 @@
         <v>113</v>
       </c>
       <c r="E244" s="15" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="F244" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="N244" s="6" t="s">
-        <v>109</v>
+        <v>169</v>
+      </c>
+      <c r="G244" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="N244" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="O244" s="6" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="P244" s="6" t="s">
-        <v>265</v>
+        <v>498</v>
       </c>
       <c r="Q244" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R244" s="4" t="s">
         <v>131</v>
@@ -16488,7 +16470,7 @@
         <v>131</v>
       </c>
       <c r="T244" s="9" t="s">
-        <v>475</v>
+        <v>178</v>
       </c>
       <c r="U244" s="10"/>
       <c r="V244" s="10"/>
@@ -16497,12 +16479,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="245" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A245" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B245" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C245" s="15" t="s">
         <v>103</v>
@@ -16513,20 +16495,17 @@
       <c r="E245" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="F245" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G245" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="N245" s="6" t="s">
-        <v>108</v>
+      <c r="N245" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="O245" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q245" s="3" t="s">
-        <v>338</v>
+        <v>109</v>
+      </c>
+      <c r="P245" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q245" s="8" t="s">
+        <v>332</v>
       </c>
       <c r="R245" s="4" t="s">
         <v>131</v>
@@ -16535,18 +16514,21 @@
         <v>131</v>
       </c>
       <c r="T245" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="X245" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="246" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+      <c r="U245" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="X245" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="246" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A246" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B246" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C246" s="15" t="s">
         <v>103</v>
@@ -16560,20 +16542,17 @@
       <c r="F246" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="G246" s="15" t="s">
-        <v>115</v>
-      </c>
       <c r="N246" s="6" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="O246" s="6" t="s">
         <v>109</v>
       </c>
       <c r="P246" s="6" t="s">
-        <v>498</v>
+        <v>265</v>
       </c>
       <c r="Q246" s="3" t="s">
-        <v>195</v>
+        <v>337</v>
       </c>
       <c r="R246" s="4" t="s">
         <v>131</v>
@@ -16582,13 +16561,13 @@
         <v>131</v>
       </c>
       <c r="T246" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="U246" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="X246" s="6" t="s">
-        <v>192</v>
+        <v>474</v>
+      </c>
+      <c r="U246" s="10"/>
+      <c r="V246" s="10"/>
+      <c r="W246" s="10"/>
+      <c r="X246" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="247" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -16596,7 +16575,7 @@
         <v>179</v>
       </c>
       <c r="B247" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C247" s="15" t="s">
         <v>103</v>
@@ -16611,22 +16590,16 @@
         <v>103</v>
       </c>
       <c r="G247" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="H247" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="N247" s="7" t="s">
-        <v>131</v>
+        <v>110</v>
+      </c>
+      <c r="N247" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="O247" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="P247" s="6" t="s">
-        <v>498</v>
+        <v>144</v>
       </c>
       <c r="Q247" s="3" t="s">
-        <v>195</v>
+        <v>338</v>
       </c>
       <c r="R247" s="4" t="s">
         <v>131</v>
@@ -16635,21 +16608,18 @@
         <v>131</v>
       </c>
       <c r="T247" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="U247" s="8" t="s">
-        <v>477</v>
+        <v>190</v>
       </c>
       <c r="X247" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A248" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B248" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C248" s="15" t="s">
         <v>103</v>
@@ -16664,19 +16634,19 @@
         <v>103</v>
       </c>
       <c r="G248" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="N248" s="6" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="O248" s="6" t="s">
         <v>109</v>
       </c>
       <c r="P248" s="6" t="s">
-        <v>265</v>
+        <v>497</v>
       </c>
       <c r="Q248" s="3" t="s">
-        <v>331</v>
+        <v>195</v>
       </c>
       <c r="R248" s="4" t="s">
         <v>131</v>
@@ -16685,18 +16655,21 @@
         <v>131</v>
       </c>
       <c r="T248" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="X248" s="13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="249" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="U248" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="X248" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="249" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B249" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C249" s="15" t="s">
         <v>103</v>
@@ -16711,22 +16684,22 @@
         <v>103</v>
       </c>
       <c r="G249" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H249" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="N249" s="6" t="s">
-        <v>167</v>
+        <v>111</v>
+      </c>
+      <c r="N249" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="O249" s="6" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="P249" s="6" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="Q249" s="3" t="s">
-        <v>332</v>
+        <v>195</v>
       </c>
       <c r="R249" s="4" t="s">
         <v>131</v>
@@ -16735,21 +16708,21 @@
         <v>131</v>
       </c>
       <c r="T249" s="9" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="U249" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="X249" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="250" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+      <c r="X249" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A250" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B250" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C250" s="15" t="s">
         <v>103</v>
@@ -16766,23 +16739,17 @@
       <c r="G250" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="H250" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="I250" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="N250" s="7" t="s">
-        <v>131</v>
+      <c r="N250" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O250" s="6" t="s">
-        <v>174</v>
+        <v>109</v>
       </c>
       <c r="P250" s="6" t="s">
-        <v>496</v>
+        <v>265</v>
       </c>
       <c r="Q250" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="R250" s="4" t="s">
         <v>131</v>
@@ -16791,23 +16758,18 @@
         <v>131</v>
       </c>
       <c r="T250" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="U250" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="V250" s="10"/>
-      <c r="W250" s="10"/>
-      <c r="X250" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="251" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+      <c r="X250" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="251" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A251" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B251" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C251" s="15" t="s">
         <v>103</v>
@@ -16825,16 +16787,16 @@
         <v>113</v>
       </c>
       <c r="H251" s="15" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="N251" s="6" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="O251" s="6" t="s">
         <v>109</v>
       </c>
       <c r="P251" s="6" t="s">
-        <v>265</v>
+        <v>495</v>
       </c>
       <c r="Q251" s="3" t="s">
         <v>332</v>
@@ -16846,21 +16808,21 @@
         <v>131</v>
       </c>
       <c r="T251" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="U251" s="10" t="s">
-        <v>105</v>
+        <v>208</v>
+      </c>
+      <c r="U251" s="8" t="s">
+        <v>207</v>
       </c>
       <c r="X251" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="252" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="252" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B252" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C252" s="15" t="s">
         <v>103</v>
@@ -16878,24 +16840,22 @@
         <v>113</v>
       </c>
       <c r="H252" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="I252" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J252" s="17"/>
-      <c r="K252" s="17"/>
-      <c r="L252" s="17"/>
-      <c r="M252" s="17"/>
-      <c r="N252" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="O252" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="P252" s="7"/>
+        <v>162</v>
+      </c>
+      <c r="I252" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="N252" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="O252" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="P252" s="6" t="s">
+        <v>495</v>
+      </c>
       <c r="Q252" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="R252" s="4" t="s">
         <v>131</v>
@@ -16904,7 +16864,7 @@
         <v>131</v>
       </c>
       <c r="T252" s="9" t="s">
-        <v>134</v>
+        <v>209</v>
       </c>
       <c r="U252" s="10" t="s">
         <v>105</v>
@@ -16915,12 +16875,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A253" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B253" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C253" s="15" t="s">
         <v>103</v>
@@ -16940,11 +16900,8 @@
       <c r="H253" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I253" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="N253" s="7" t="s">
-        <v>131</v>
+      <c r="N253" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="O253" s="6" t="s">
         <v>109</v>
@@ -16953,7 +16910,7 @@
         <v>265</v>
       </c>
       <c r="Q253" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R253" s="4" t="s">
         <v>131</v>
@@ -16962,23 +16919,21 @@
         <v>131</v>
       </c>
       <c r="T253" s="9" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="U253" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="V253" s="10"/>
-      <c r="W253" s="10"/>
-      <c r="X253" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X253" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="254" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A254" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B254" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C254" s="15" t="s">
         <v>103</v>
@@ -16998,23 +16953,22 @@
       <c r="H254" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I254" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="J254" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="N254" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="O254" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="P254" s="6" t="s">
-        <v>380</v>
-      </c>
+      <c r="I254" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J254" s="17"/>
+      <c r="K254" s="17"/>
+      <c r="L254" s="17"/>
+      <c r="M254" s="17"/>
+      <c r="N254" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="O254" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="P254" s="7"/>
       <c r="Q254" s="3" t="s">
-        <v>451</v>
+        <v>333</v>
       </c>
       <c r="R254" s="4" t="s">
         <v>131</v>
@@ -17023,7 +16977,7 @@
         <v>131</v>
       </c>
       <c r="T254" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="U254" s="10" t="s">
         <v>105</v>
@@ -17034,12 +16988,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="255" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A255" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B255" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C255" s="15" t="s">
         <v>103</v>
@@ -17062,20 +17016,17 @@
       <c r="I255" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="J255" s="15" t="s">
-        <v>139</v>
-      </c>
       <c r="N255" s="7" t="s">
         <v>131</v>
       </c>
       <c r="O255" s="6" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="P255" s="6" t="s">
-        <v>504</v>
+        <v>265</v>
       </c>
       <c r="Q255" s="3" t="s">
-        <v>451</v>
+        <v>333</v>
       </c>
       <c r="R255" s="4" t="s">
         <v>131</v>
@@ -17084,7 +17035,7 @@
         <v>131</v>
       </c>
       <c r="T255" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="U255" s="10" t="s">
         <v>105</v>
@@ -17095,91 +17046,143 @@
         <v>105</v>
       </c>
     </row>
-    <row r="256" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A256" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B256" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="C256" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D256" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E256" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F256" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G256" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H256" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="I256" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="J256" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="N256" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="O256" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="P256" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q256" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="R256" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S256" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T256" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="U256" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="V256" s="10"/>
+      <c r="W256" s="10"/>
+      <c r="X256" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="257" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A257" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B257" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="C257" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D257" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E257" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F257" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G257" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H257" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="I257" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="J257" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="N257" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="O257" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="P257" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q257" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="R257" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S257" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T257" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="U257" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="V257" s="10"/>
+      <c r="W257" s="10"/>
+      <c r="X257" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="258" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A258" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B258" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N256" s="6" t="s">
+      <c r="N258" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="O256" s="6" t="s">
+      <c r="O258" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="P256" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="Q256" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="R256" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="S256" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="T256" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="U256" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="V256" s="8" t="s">
-        <v>480</v>
-      </c>
-      <c r="X256" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="257" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A257" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B257" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="N257" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="O257" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="P257" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="Q257" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="R257" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="S257" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="T257" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="X257" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="258" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A258" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B258" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="N258" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="O258" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="P258" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="Q258" s="8" t="s">
         <v>341</v>
@@ -17187,60 +17190,60 @@
       <c r="R258" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="S258" s="8" t="s">
-        <v>341</v>
+      <c r="S258" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="T258" s="9" t="s">
-        <v>485</v>
+        <v>477</v>
+      </c>
+      <c r="U258" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="V258" s="8" t="s">
+        <v>479</v>
       </c>
       <c r="X258" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="259" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B259" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C259" s="15" t="s">
-        <v>482</v>
-      </c>
-      <c r="N259" s="7" t="s">
-        <v>131</v>
+        <v>51</v>
+      </c>
+      <c r="N259" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="O259" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P259" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="Q259" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="R259" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="S259" s="3" t="s">
-        <v>483</v>
+        <v>507</v>
+      </c>
+      <c r="Q259" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="R259" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="S259" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="T259" s="9" t="s">
-        <v>484</v>
-      </c>
-      <c r="U259" s="8" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="X259" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="260" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B260" s="15" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="N260" s="6" t="s">
         <v>145</v>
@@ -17252,36 +17255,30 @@
         <v>505</v>
       </c>
       <c r="Q260" s="8" t="s">
-        <v>493</v>
-      </c>
-      <c r="R260" s="4" t="s">
-        <v>131</v>
+        <v>341</v>
+      </c>
+      <c r="R260" s="8" t="s">
+        <v>341</v>
       </c>
       <c r="S260" s="8" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
       <c r="T260" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="U260" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="W260" s="8" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="X260" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="261" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" s="16" t="s">
         <v>179</v>
       </c>
       <c r="B261" s="15" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C261" s="15" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="N261" s="7" t="s">
         <v>131</v>
@@ -17293,24 +17290,100 @@
         <v>505</v>
       </c>
       <c r="Q261" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="R261" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="S261" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="T261" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="U261" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="X261" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="262" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A262" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B262" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N262" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="O262" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="P262" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q262" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="R262" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S262" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="T262" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="U262" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="R261" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="S261" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="T261" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="U261" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="W261" s="8" t="s">
-        <v>495</v>
-      </c>
-      <c r="X261" s="6" t="s">
+      <c r="W262" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="X262" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="263" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A263" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B263" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C263" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="N263" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="O263" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="P263" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="Q263" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="R263" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S263" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="T263" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="U263" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="W263" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="X263" s="6" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>